<commit_message>
Vytvorenie statistiky pre dobu obsluhy
</commit_message>
<xml_diff>
--- a/data-supermarket.xlsx
+++ b/data-supermarket.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documents\vysokaSkola\MAS\semestralna praca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="doba_obsluhypokladne_1" localSheetId="0">'Obsluha na pokladni'!$B$4:$E$102</definedName>
+    <definedName name="New_Text_Document" localSheetId="0">'Obsluha na pokladni'!$G$4:$G$103</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,6 +40,13 @@
         <textField position="10"/>
         <textField position="19"/>
         <textField position="31"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="New Text Document" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\New Text Document.txt">
+      <textFields>
+        <textField/>
       </textFields>
     </textPr>
   </connection>
@@ -111,9 +119,6 @@
     <t>DOBA OBSLUHY NA POKLADNI</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
@@ -152,14 +157,16 @@
   <si>
     <t>Count</t>
   </si>
+  <si>
+    <t>Doba obsluhy na pokladni</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
-    <numFmt numFmtId="167" formatCode="[ss]"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -489,11 +496,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -502,6 +505,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,6 +532,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -793,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +815,7 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="9" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,14 +826,14 @@
     </row>
     <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="36"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -841,10 +853,10 @@
       <c r="E3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="37" t="s">
         <v>19</v>
       </c>
     </row>
@@ -864,18 +876,17 @@
       <c r="E4" s="28">
         <v>0.4880902777777778</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="36">
         <f>E4-C4</f>
         <v>5.4398148148154801E-4</v>
       </c>
-      <c r="G4" s="38">
-        <f>TIME(E4,E4,E4)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="42"/>
+      <c r="G4" s="42">
+        <v>47</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -893,16 +904,15 @@
       <c r="E5" s="28">
         <v>0.48927083333333332</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <f t="shared" ref="F5:F68" si="0">E5-C5</f>
         <v>1.1458333333333459E-3</v>
       </c>
-      <c r="G5" s="38">
-        <f t="shared" ref="G5:H68" si="1">F5</f>
-        <v>1.1458333333333459E-3</v>
-      </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
+      <c r="G5" s="42">
+        <v>99</v>
+      </c>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
@@ -920,19 +930,18 @@
       <c r="E6" s="28">
         <v>0.48947916666666669</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <f t="shared" si="0"/>
         <v>1.8518518518523264E-4</v>
       </c>
-      <c r="G6" s="38">
-        <f t="shared" si="1"/>
-        <v>1.8518518518523264E-4</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="40">
-        <v>5.0694444444444875E-4</v>
+      <c r="G6" s="42">
+        <v>16</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="38">
+        <v>43.8</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -951,19 +960,18 @@
       <c r="E7" s="28">
         <v>0.48979166666666668</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <f t="shared" si="0"/>
         <v>2.777777777778212E-4</v>
       </c>
-      <c r="G7" s="38">
-        <f t="shared" si="1"/>
-        <v>2.777777777778212E-4</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="40">
-        <v>2.7822557122696743E-5</v>
+      <c r="G7" s="42">
+        <v>24</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="38">
+        <v>2.4038689354009835</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,19 +990,18 @@
       <c r="E8" s="28">
         <v>0.49079861111111112</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="36">
         <f t="shared" si="0"/>
         <v>9.6064814814816879E-4</v>
       </c>
-      <c r="G8" s="38">
-        <f t="shared" si="1"/>
-        <v>9.6064814814816879E-4</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="40">
-        <v>4.8611111111107608E-4</v>
+      <c r="G8" s="42">
+        <v>83</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="38">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1013,19 +1020,18 @@
       <c r="E9" s="28">
         <v>0.49094907407407407</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="36">
         <f t="shared" si="0"/>
         <v>5.7870370370360913E-5</v>
       </c>
-      <c r="G9" s="38">
-        <f t="shared" si="1"/>
-        <v>5.7870370370360913E-5</v>
-      </c>
-      <c r="I9" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="40">
-        <v>4.861111111111871E-4</v>
+      <c r="G9" s="42">
+        <v>5</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="38">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1044,19 +1050,18 @@
       <c r="E10" s="28">
         <v>0.49131944444444442</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <f t="shared" si="0"/>
         <v>3.3564814814807109E-4</v>
       </c>
-      <c r="G10" s="38">
-        <f t="shared" si="1"/>
-        <v>3.3564814814807109E-4</v>
-      </c>
-      <c r="I10" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="40">
-        <v>2.7822557122696742E-4</v>
+      <c r="G10" s="42">
+        <v>29</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="38">
+        <v>24.038689354009836</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1075,19 +1080,18 @@
       <c r="E11" s="28">
         <v>0.49163194444444441</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <f t="shared" si="0"/>
         <v>2.3148148148144365E-4</v>
       </c>
-      <c r="G11" s="38">
-        <f t="shared" si="1"/>
-        <v>2.3148148148144365E-4</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="40">
-        <v>7.7409468484572321E-8</v>
+      <c r="G11" s="42">
+        <v>20</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="38">
+        <v>577.85858585858591</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1106,19 +1110,18 @@
       <c r="E12" s="28">
         <v>0.49217592592592596</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="36">
         <f t="shared" si="0"/>
         <v>4.0509259259263741E-4</v>
       </c>
-      <c r="G12" s="38">
-        <f t="shared" si="1"/>
-        <v>4.0509259259263741E-4</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="40">
-        <v>2.4605882226919857</v>
+      <c r="G12" s="42">
+        <v>35</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="38">
+        <v>2.4605882226919138</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1137,19 +1140,18 @@
       <c r="E13" s="28">
         <v>0.49265046296296294</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="36">
         <f t="shared" si="0"/>
         <v>3.0092592592589895E-4</v>
       </c>
-      <c r="G13" s="38">
-        <f t="shared" si="1"/>
-        <v>3.0092592592589895E-4</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="40">
-        <v>1.0425245334883952</v>
+      <c r="G13" s="42">
+        <v>26</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="38">
+        <v>1.0425245334884037</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,19 +1170,18 @@
       <c r="E14" s="28">
         <v>0.49437500000000001</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="36">
         <f t="shared" si="0"/>
         <v>1.6898148148148384E-3</v>
       </c>
-      <c r="G14" s="38">
-        <f t="shared" si="1"/>
-        <v>1.6898148148148384E-3</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="40">
-        <v>1.6898148148148384E-3</v>
+      <c r="G14" s="42">
+        <v>146</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="38">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1199,18 +1200,17 @@
       <c r="E15" s="28">
         <v>0.49501157407407409</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="36">
         <f t="shared" si="0"/>
         <v>2.8935185185186008E-4</v>
       </c>
-      <c r="G15" s="38">
-        <f t="shared" si="1"/>
-        <v>2.8935185185186008E-4</v>
-      </c>
-      <c r="I15" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="40">
+      <c r="G15" s="42">
+        <v>25</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1230,19 +1230,18 @@
       <c r="E16" s="28">
         <v>0.49576388888888889</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="36">
         <f t="shared" si="0"/>
         <v>6.9444444444449749E-4</v>
       </c>
-      <c r="G16" s="38">
-        <f t="shared" si="1"/>
-        <v>6.9444444444449749E-4</v>
-      </c>
-      <c r="I16" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="40">
-        <v>1.6898148148148384E-3</v>
+      <c r="G16" s="42">
+        <v>60</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="38">
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1261,19 +1260,18 @@
       <c r="E17" s="28">
         <v>0.49619212962962966</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="36">
         <f t="shared" si="0"/>
         <v>4.0509259259263741E-4</v>
       </c>
-      <c r="G17" s="38">
-        <f t="shared" si="1"/>
-        <v>4.0509259259263741E-4</v>
-      </c>
-      <c r="I17" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="40">
-        <v>5.0694444444444875E-2</v>
+      <c r="G17" s="42">
+        <v>35</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="38">
+        <v>4380</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1292,18 +1290,17 @@
       <c r="E18" s="28">
         <v>0.49652777777777773</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="36">
         <f t="shared" si="0"/>
         <v>3.0092592592589895E-4</v>
       </c>
-      <c r="G18" s="38">
-        <f t="shared" si="1"/>
-        <v>3.0092592592589895E-4</v>
-      </c>
-      <c r="I18" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="41">
+      <c r="G18" s="42">
+        <v>26</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="39">
         <v>100</v>
       </c>
     </row>
@@ -1323,13 +1320,12 @@
       <c r="E19" s="28">
         <v>0.4968981481481482</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="36">
         <f t="shared" si="0"/>
         <v>3.5879629629631538E-4</v>
       </c>
-      <c r="G19" s="38">
-        <f t="shared" si="1"/>
-        <v>3.5879629629631538E-4</v>
+      <c r="G19" s="42">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,13 +1344,12 @@
       <c r="E20" s="28">
         <v>0.4979513888888889</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="36">
         <f t="shared" si="0"/>
         <v>3.3564814814818211E-4</v>
       </c>
-      <c r="G20" s="38">
-        <f t="shared" si="1"/>
-        <v>3.3564814814818211E-4</v>
+      <c r="G20" s="42">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1373,13 +1368,12 @@
       <c r="E21" s="28">
         <v>0.49881944444444443</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="36">
         <f t="shared" si="0"/>
         <v>8.4490740740739145E-4</v>
       </c>
-      <c r="G21" s="38">
-        <f t="shared" si="1"/>
-        <v>8.4490740740739145E-4</v>
+      <c r="G21" s="42">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1398,13 +1392,12 @@
       <c r="E22" s="28">
         <v>0.49958333333333332</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="36">
         <f t="shared" si="0"/>
         <v>7.5231481481480289E-4</v>
       </c>
-      <c r="G22" s="38">
-        <f t="shared" si="1"/>
-        <v>7.5231481481480289E-4</v>
+      <c r="G22" s="42">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1423,13 +1416,12 @@
       <c r="E23" s="28">
         <v>0.50017361111111114</v>
       </c>
-      <c r="F23" s="37">
+      <c r="F23" s="36">
         <f t="shared" si="0"/>
         <v>5.6712962962962576E-4</v>
       </c>
-      <c r="G23" s="38">
-        <f t="shared" si="1"/>
-        <v>5.6712962962962576E-4</v>
+      <c r="G23" s="42">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1448,13 +1440,12 @@
       <c r="E24" s="28">
         <v>0.5006828703703704</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="36">
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G24" s="38">
-        <f t="shared" si="1"/>
-        <v>4.861111111111871E-4</v>
+      <c r="G24" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1473,13 +1464,12 @@
       <c r="E25" s="28">
         <v>0.5018055555555555</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="36">
         <f t="shared" si="0"/>
         <v>6.8287037037029208E-4</v>
       </c>
-      <c r="G25" s="38">
-        <f t="shared" si="1"/>
-        <v>6.8287037037029208E-4</v>
+      <c r="G25" s="42">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1498,13 +1488,12 @@
       <c r="E26" s="28">
         <v>0.50298611111111113</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="36">
         <f t="shared" si="0"/>
         <v>1.0185185185185297E-3</v>
       </c>
-      <c r="G26" s="38">
-        <f t="shared" si="1"/>
-        <v>1.0185185185185297E-3</v>
+      <c r="G26" s="42">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1523,13 +1512,12 @@
       <c r="E27" s="28">
         <v>0.50348379629629625</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="36">
         <f t="shared" si="0"/>
         <v>4.7453703703692618E-4</v>
       </c>
-      <c r="G27" s="38">
-        <f t="shared" si="1"/>
-        <v>4.7453703703692618E-4</v>
+      <c r="G27" s="42">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1548,13 +1536,12 @@
       <c r="E28" s="28">
         <v>0.50394675925925925</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="36">
         <f t="shared" si="0"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="G28" s="38">
-        <f t="shared" si="1"/>
-        <v>4.3981481481480955E-4</v>
+      <c r="G28" s="42">
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1573,13 +1560,12 @@
       <c r="E29" s="28">
         <v>0.50457175925925923</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="36">
         <f t="shared" si="0"/>
         <v>5.7870370370372015E-4</v>
       </c>
-      <c r="G29" s="38">
-        <f t="shared" si="1"/>
-        <v>5.7870370370372015E-4</v>
+      <c r="G29" s="42">
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1598,13 +1584,12 @@
       <c r="E30" s="28">
         <v>0.50496527777777778</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="36">
         <f t="shared" si="0"/>
         <v>3.4722222222216548E-4</v>
       </c>
-      <c r="G30" s="38">
-        <f t="shared" si="1"/>
-        <v>3.4722222222216548E-4</v>
+      <c r="G30" s="42">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1623,13 +1608,12 @@
       <c r="E31" s="28">
         <v>0.50564814814814818</v>
       </c>
-      <c r="F31" s="37">
+      <c r="F31" s="36">
         <f t="shared" si="0"/>
         <v>6.5972222222221433E-4</v>
       </c>
-      <c r="G31" s="38">
-        <f t="shared" si="1"/>
-        <v>6.5972222222221433E-4</v>
+      <c r="G31" s="42">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1648,13 +1632,12 @@
       <c r="E32" s="28">
         <v>0.50593750000000004</v>
       </c>
-      <c r="F32" s="37">
+      <c r="F32" s="36">
         <f t="shared" si="0"/>
         <v>2.5462962962974345E-4</v>
       </c>
-      <c r="G32" s="38">
-        <f t="shared" si="1"/>
-        <v>2.5462962962974345E-4</v>
+      <c r="G32" s="42">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,13 +1656,12 @@
       <c r="E33" s="28">
         <v>0.5064467592592593</v>
       </c>
-      <c r="F33" s="37">
+      <c r="F33" s="36">
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G33" s="38">
-        <f t="shared" si="1"/>
-        <v>4.861111111111871E-4</v>
+      <c r="G33" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1698,13 +1680,12 @@
       <c r="E34" s="28">
         <v>0.50706018518518514</v>
       </c>
-      <c r="F34" s="37">
+      <c r="F34" s="36">
         <f t="shared" si="0"/>
         <v>6.018518518517979E-4</v>
       </c>
-      <c r="G34" s="38">
-        <f t="shared" si="1"/>
-        <v>6.018518518517979E-4</v>
+      <c r="G34" s="42">
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1723,13 +1704,12 @@
       <c r="E35" s="28">
         <v>0.5074305555555555</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="36">
         <f t="shared" si="0"/>
         <v>3.1249999999993783E-4</v>
       </c>
-      <c r="G35" s="38">
-        <f t="shared" si="1"/>
-        <v>3.1249999999993783E-4</v>
+      <c r="G35" s="42">
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,13 +1728,12 @@
       <c r="E36" s="28">
         <v>0.50813657407407409</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="36">
         <f t="shared" si="0"/>
         <v>6.9444444444444198E-4</v>
       </c>
-      <c r="G36" s="38">
-        <f t="shared" si="1"/>
-        <v>6.9444444444444198E-4</v>
+      <c r="G36" s="42">
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,13 +1752,12 @@
       <c r="E37" s="28">
         <v>0.50854166666666667</v>
       </c>
-      <c r="F37" s="37">
+      <c r="F37" s="36">
         <f t="shared" si="0"/>
         <v>3.8194444444450415E-4</v>
       </c>
-      <c r="G37" s="38">
-        <f t="shared" si="1"/>
-        <v>3.8194444444450415E-4</v>
+      <c r="G37" s="42">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1798,13 +1776,12 @@
       <c r="E38" s="28">
         <v>0.50901620370370371</v>
       </c>
-      <c r="F38" s="37">
+      <c r="F38" s="36">
         <f t="shared" si="0"/>
         <v>4.6296296296299833E-4</v>
       </c>
-      <c r="G38" s="38">
-        <f t="shared" si="1"/>
-        <v>4.6296296296299833E-4</v>
+      <c r="G38" s="42">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,13 +1800,12 @@
       <c r="E39" s="28">
         <v>0.50951388888888893</v>
       </c>
-      <c r="F39" s="37">
+      <c r="F39" s="36">
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G39" s="38">
-        <f t="shared" si="1"/>
-        <v>4.861111111111871E-4</v>
+      <c r="G39" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1848,13 +1824,12 @@
       <c r="E40" s="28">
         <v>0.51075231481481487</v>
       </c>
-      <c r="F40" s="37">
+      <c r="F40" s="36">
         <f t="shared" si="0"/>
         <v>1.1574074074074403E-3</v>
       </c>
-      <c r="G40" s="38">
-        <f t="shared" si="1"/>
-        <v>1.1574074074074403E-3</v>
+      <c r="G40" s="42">
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1873,13 +1848,12 @@
       <c r="E41" s="28">
         <v>0.51107638888888884</v>
       </c>
-      <c r="F41" s="37">
+      <c r="F41" s="36">
         <f t="shared" si="0"/>
         <v>2.0833333333325488E-4</v>
       </c>
-      <c r="G41" s="38">
-        <f t="shared" si="1"/>
-        <v>2.0833333333325488E-4</v>
+      <c r="G41" s="42">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1898,13 +1872,12 @@
       <c r="E42" s="28">
         <v>0.51168981481481479</v>
       </c>
-      <c r="F42" s="37">
+      <c r="F42" s="36">
         <f t="shared" si="0"/>
         <v>6.018518518517979E-4</v>
       </c>
-      <c r="G42" s="38">
-        <f t="shared" si="1"/>
-        <v>6.018518518517979E-4</v>
+      <c r="G42" s="42">
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1923,13 +1896,12 @@
       <c r="E43" s="28">
         <v>0.51178240740740744</v>
       </c>
-      <c r="F43" s="37">
+      <c r="F43" s="36">
         <f t="shared" si="0"/>
         <v>8.1018518518494176E-5</v>
       </c>
-      <c r="G43" s="38">
-        <f t="shared" si="1"/>
-        <v>8.1018518518494176E-5</v>
+      <c r="G43" s="42">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1948,13 +1920,12 @@
       <c r="E44" s="28">
         <v>0.51230324074074074</v>
       </c>
-      <c r="F44" s="37">
+      <c r="F44" s="36">
         <f t="shared" si="0"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="G44" s="38">
-        <f t="shared" si="1"/>
-        <v>5.0925925925926485E-4</v>
+      <c r="G44" s="42">
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1973,13 +1944,12 @@
       <c r="E45" s="28">
         <v>0.51292824074074073</v>
       </c>
-      <c r="F45" s="37">
+      <c r="F45" s="36">
         <f t="shared" si="0"/>
         <v>6.134259259259478E-4</v>
       </c>
-      <c r="G45" s="38">
-        <f t="shared" si="1"/>
-        <v>6.134259259259478E-4</v>
+      <c r="G45" s="42">
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1998,13 +1968,12 @@
       <c r="E46" s="28">
         <v>0.51351851851851849</v>
       </c>
-      <c r="F46" s="37">
+      <c r="F46" s="36">
         <f t="shared" si="0"/>
         <v>5.324074074073426E-4</v>
       </c>
-      <c r="G46" s="38">
-        <f t="shared" si="1"/>
-        <v>5.324074074073426E-4</v>
+      <c r="G46" s="42">
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2023,13 +1992,12 @@
       <c r="E47" s="28">
         <v>0.51439814814814822</v>
       </c>
-      <c r="F47" s="37">
+      <c r="F47" s="36">
         <f t="shared" si="0"/>
         <v>8.4490740740750248E-4</v>
       </c>
-      <c r="G47" s="38">
-        <f t="shared" si="1"/>
-        <v>8.4490740740750248E-4</v>
+      <c r="G47" s="42">
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2048,13 +2016,12 @@
       <c r="E48" s="28">
         <v>0.51508101851851851</v>
       </c>
-      <c r="F48" s="37">
+      <c r="F48" s="36">
         <f t="shared" si="0"/>
         <v>6.712962962962532E-4</v>
       </c>
-      <c r="G48" s="38">
-        <f t="shared" si="1"/>
-        <v>6.712962962962532E-4</v>
+      <c r="G48" s="42">
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2073,13 +2040,12 @@
       <c r="E49" s="28">
         <v>0.51538194444444441</v>
       </c>
-      <c r="F49" s="37">
+      <c r="F49" s="36">
         <f t="shared" si="0"/>
         <v>2.7777777777771018E-4</v>
       </c>
-      <c r="G49" s="38">
-        <f t="shared" si="1"/>
-        <v>2.7777777777771018E-4</v>
+      <c r="G49" s="42">
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2098,13 +2064,12 @@
       <c r="E50" s="28">
         <v>0.51553240740740736</v>
       </c>
-      <c r="F50" s="37">
+      <c r="F50" s="36">
         <f t="shared" si="0"/>
         <v>1.388888888889106E-4</v>
       </c>
-      <c r="G50" s="38">
-        <f t="shared" si="1"/>
-        <v>1.388888888889106E-4</v>
+      <c r="G50" s="42">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2123,13 +2088,12 @@
       <c r="E51" s="28">
         <v>0.5157870370370371</v>
       </c>
-      <c r="F51" s="37">
+      <c r="F51" s="36">
         <f t="shared" si="0"/>
         <v>2.4305555555559355E-4</v>
       </c>
-      <c r="G51" s="38">
-        <f t="shared" si="1"/>
-        <v>2.4305555555559355E-4</v>
+      <c r="G51" s="42">
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,13 +2112,12 @@
       <c r="E52" s="28">
         <v>0.51599537037037035</v>
       </c>
-      <c r="F52" s="37">
+      <c r="F52" s="36">
         <f t="shared" si="0"/>
         <v>1.7361111111113825E-4</v>
       </c>
-      <c r="G52" s="38">
-        <f t="shared" si="1"/>
-        <v>1.7361111111113825E-4</v>
+      <c r="G52" s="42">
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2173,13 +2136,12 @@
       <c r="E53" s="28">
         <v>0.51684027777777775</v>
       </c>
-      <c r="F53" s="37">
+      <c r="F53" s="36">
         <f t="shared" si="0"/>
         <v>8.3333333333324155E-4</v>
       </c>
-      <c r="G53" s="38">
-        <f t="shared" si="1"/>
-        <v>8.3333333333324155E-4</v>
+      <c r="G53" s="42">
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2198,13 +2160,12 @@
       <c r="E54" s="28">
         <v>0.51730324074074074</v>
       </c>
-      <c r="F54" s="37">
+      <c r="F54" s="36">
         <f t="shared" si="0"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="G54" s="38">
-        <f t="shared" si="1"/>
-        <v>4.3981481481480955E-4</v>
+      <c r="G54" s="42">
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,13 +2184,12 @@
       <c r="E55" s="28">
         <v>0.51778935185185182</v>
       </c>
-      <c r="F55" s="37">
+      <c r="F55" s="36">
         <f t="shared" si="0"/>
         <v>4.8611111111107608E-4</v>
       </c>
-      <c r="G55" s="38">
-        <f t="shared" si="1"/>
-        <v>4.8611111111107608E-4</v>
+      <c r="G55" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2248,13 +2208,12 @@
       <c r="E56" s="28">
         <v>0.51857638888888891</v>
       </c>
-      <c r="F56" s="37">
+      <c r="F56" s="36">
         <f t="shared" si="0"/>
         <v>7.2916666666666963E-4</v>
       </c>
-      <c r="G56" s="38">
-        <f t="shared" si="1"/>
-        <v>7.2916666666666963E-4</v>
+      <c r="G56" s="42">
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2273,13 +2232,12 @@
       <c r="E57" s="28">
         <v>0.51914351851851859</v>
       </c>
-      <c r="F57" s="37">
+      <c r="F57" s="36">
         <f t="shared" si="0"/>
         <v>5.555555555556424E-4</v>
       </c>
-      <c r="G57" s="38">
-        <f t="shared" si="1"/>
-        <v>5.555555555556424E-4</v>
+      <c r="G57" s="42">
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2298,13 +2256,12 @@
       <c r="E58" s="28">
         <v>0.51954861111111106</v>
       </c>
-      <c r="F58" s="37">
+      <c r="F58" s="36">
         <f t="shared" si="0"/>
         <v>3.5879629629631538E-4</v>
       </c>
-      <c r="G58" s="38">
-        <f t="shared" si="1"/>
-        <v>3.5879629629631538E-4</v>
+      <c r="G58" s="42">
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,13 +2280,12 @@
       <c r="E59" s="28">
         <v>0.52023148148148146</v>
       </c>
-      <c r="F59" s="37">
+      <c r="F59" s="36">
         <f t="shared" si="0"/>
         <v>6.3657407407402555E-4</v>
       </c>
-      <c r="G59" s="38">
-        <f t="shared" si="1"/>
-        <v>6.3657407407402555E-4</v>
+      <c r="G59" s="42">
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2348,13 +2304,12 @@
       <c r="E60" s="28">
         <v>0.52069444444444446</v>
       </c>
-      <c r="F60" s="37">
+      <c r="F60" s="36">
         <f t="shared" si="0"/>
         <v>4.2824074074077068E-4</v>
       </c>
-      <c r="G60" s="38">
-        <f t="shared" si="1"/>
-        <v>4.2824074074077068E-4</v>
+      <c r="G60" s="42">
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2373,13 +2328,12 @@
       <c r="E61" s="28">
         <v>0.52143518518518517</v>
       </c>
-      <c r="F61" s="37">
+      <c r="F61" s="36">
         <f t="shared" si="0"/>
         <v>7.1759259259263075E-4</v>
       </c>
-      <c r="G61" s="38">
-        <f t="shared" si="1"/>
-        <v>7.1759259259263075E-4</v>
+      <c r="G61" s="42">
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2398,13 +2352,12 @@
       <c r="E62" s="28">
         <v>0.52197916666666666</v>
       </c>
-      <c r="F62" s="37">
+      <c r="F62" s="36">
         <f t="shared" si="0"/>
         <v>5.3240740740745363E-4</v>
       </c>
-      <c r="G62" s="38">
-        <f t="shared" si="1"/>
-        <v>5.3240740740745363E-4</v>
+      <c r="G62" s="42">
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2423,13 +2376,12 @@
       <c r="E63" s="28">
         <v>0.52253472222222219</v>
       </c>
-      <c r="F63" s="37">
+      <c r="F63" s="36">
         <f t="shared" si="0"/>
         <v>4.9768518518522598E-4</v>
       </c>
-      <c r="G63" s="38">
-        <f t="shared" si="1"/>
-        <v>4.9768518518522598E-4</v>
+      <c r="G63" s="42">
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2448,13 +2400,12 @@
       <c r="E64" s="28">
         <v>0.52303240740740742</v>
       </c>
-      <c r="F64" s="37">
+      <c r="F64" s="36">
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G64" s="38">
-        <f t="shared" si="1"/>
-        <v>4.861111111111871E-4</v>
+      <c r="G64" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2473,13 +2424,12 @@
       <c r="E65" s="28">
         <v>0.52350694444444446</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="36">
         <f t="shared" si="0"/>
         <v>4.6296296296299833E-4</v>
       </c>
-      <c r="G65" s="38">
-        <f t="shared" si="1"/>
-        <v>4.6296296296299833E-4</v>
+      <c r="G65" s="42">
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2498,13 +2448,12 @@
       <c r="E66" s="28">
         <v>0.52410879629629636</v>
       </c>
-      <c r="F66" s="37">
+      <c r="F66" s="36">
         <f t="shared" si="0"/>
         <v>5.9027777777787005E-4</v>
       </c>
-      <c r="G66" s="38">
-        <f t="shared" si="1"/>
-        <v>5.9027777777787005E-4</v>
+      <c r="G66" s="42">
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2523,13 +2472,12 @@
       <c r="E67" s="28">
         <v>0.52515046296296297</v>
       </c>
-      <c r="F67" s="37">
+      <c r="F67" s="36">
         <f t="shared" si="0"/>
         <v>1.0300925925925686E-3</v>
       </c>
-      <c r="G67" s="38">
-        <f t="shared" si="1"/>
-        <v>1.0300925925925686E-3</v>
+      <c r="G67" s="42">
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2548,13 +2496,12 @@
       <c r="E68" s="28">
         <v>0.5292824074074074</v>
       </c>
-      <c r="F68" s="37">
+      <c r="F68" s="36">
         <f t="shared" si="0"/>
         <v>8.796296296296191E-4</v>
       </c>
-      <c r="G68" s="38">
-        <f t="shared" si="1"/>
-        <v>8.796296296296191E-4</v>
+      <c r="G68" s="42">
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2573,13 +2520,12 @@
       <c r="E69" s="28">
         <v>0.53020833333333328</v>
       </c>
-      <c r="F69" s="37">
-        <f t="shared" ref="F69:F103" si="2">E69-C69</f>
+      <c r="F69" s="36">
+        <f t="shared" ref="F69:F103" si="1">E69-C69</f>
         <v>3.4722222222216548E-4</v>
       </c>
-      <c r="G69" s="38">
-        <f t="shared" ref="G69:H103" si="3">F69</f>
-        <v>3.4722222222216548E-4</v>
+      <c r="G69" s="42">
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2598,13 +2544,12 @@
       <c r="E70" s="28">
         <v>0.53033564814814815</v>
       </c>
-      <c r="F70" s="37">
-        <f t="shared" si="2"/>
+      <c r="F70" s="36">
+        <f t="shared" si="1"/>
         <v>8.1018518518494176E-5</v>
       </c>
-      <c r="G70" s="38">
-        <f t="shared" si="3"/>
-        <v>8.1018518518494176E-5</v>
+      <c r="G70" s="42">
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2623,13 +2568,12 @@
       <c r="E71" s="28">
         <v>0.53039351851851857</v>
       </c>
-      <c r="F71" s="37">
-        <f t="shared" si="2"/>
+      <c r="F71" s="36">
+        <f t="shared" si="1"/>
         <v>1.1574074074149898E-5</v>
       </c>
-      <c r="G71" s="38">
-        <f t="shared" si="3"/>
-        <v>1.1574074074149898E-5</v>
+      <c r="G71" s="42">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2648,13 +2592,12 @@
       <c r="E72" s="28">
         <v>0.5307291666666667</v>
       </c>
-      <c r="F72" s="37">
-        <f t="shared" si="2"/>
+      <c r="F72" s="36">
+        <f t="shared" si="1"/>
         <v>2.8935185185186008E-4</v>
       </c>
-      <c r="G72" s="38">
-        <f t="shared" si="3"/>
-        <v>2.8935185185186008E-4</v>
+      <c r="G72" s="42">
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,13 +2616,12 @@
       <c r="E73" s="28">
         <v>0.53234953703703702</v>
       </c>
-      <c r="F73" s="37">
-        <f t="shared" si="2"/>
+      <c r="F73" s="36">
+        <f t="shared" si="1"/>
         <v>8.9120370370365798E-4</v>
       </c>
-      <c r="G73" s="38">
-        <f t="shared" si="3"/>
-        <v>8.9120370370365798E-4</v>
+      <c r="G73" s="42">
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2698,13 +2640,12 @@
       <c r="E74" s="28">
         <v>0.53288194444444448</v>
       </c>
-      <c r="F74" s="37">
-        <f t="shared" si="2"/>
+      <c r="F74" s="36">
+        <f t="shared" si="1"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="G74" s="38">
-        <f t="shared" si="3"/>
-        <v>5.0925925925926485E-4</v>
+      <c r="G74" s="42">
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2723,13 +2664,12 @@
       <c r="E75" s="28">
         <v>0.53340277777777778</v>
       </c>
-      <c r="F75" s="37">
-        <f t="shared" si="2"/>
+      <c r="F75" s="36">
+        <f t="shared" si="1"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="G75" s="38">
-        <f t="shared" si="3"/>
-        <v>5.0925925925926485E-4</v>
+      <c r="G75" s="42">
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2748,13 +2688,12 @@
       <c r="E76" s="28">
         <v>0.53384259259259259</v>
       </c>
-      <c r="F76" s="37">
-        <f t="shared" si="2"/>
+      <c r="F76" s="36">
+        <f t="shared" si="1"/>
         <v>4.2824074074077068E-4</v>
       </c>
-      <c r="G76" s="38">
-        <f t="shared" si="3"/>
-        <v>4.2824074074077068E-4</v>
+      <c r="G76" s="42">
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2773,13 +2712,12 @@
       <c r="E77" s="28">
         <v>0.53451388888888884</v>
       </c>
-      <c r="F77" s="37">
-        <f t="shared" si="2"/>
+      <c r="F77" s="36">
+        <f t="shared" si="1"/>
         <v>6.2499999999998668E-4</v>
       </c>
-      <c r="G77" s="38">
-        <f t="shared" si="3"/>
-        <v>6.2499999999998668E-4</v>
+      <c r="G77" s="42">
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,13 +2736,12 @@
       <c r="E78" s="28">
         <v>0.53498842592592599</v>
       </c>
-      <c r="F78" s="37">
-        <f t="shared" si="2"/>
+      <c r="F78" s="36">
+        <f t="shared" si="1"/>
         <v>3.8194444444450415E-4</v>
       </c>
-      <c r="G78" s="38">
-        <f t="shared" si="3"/>
-        <v>3.8194444444450415E-4</v>
+      <c r="G78" s="42">
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2823,13 +2760,12 @@
       <c r="E79" s="28">
         <v>0.5352662037037037</v>
       </c>
-      <c r="F79" s="37">
-        <f t="shared" si="2"/>
+      <c r="F79" s="36">
+        <f t="shared" si="1"/>
         <v>2.7777777777771018E-4</v>
       </c>
-      <c r="G79" s="38">
-        <f t="shared" si="3"/>
-        <v>2.7777777777771018E-4</v>
+      <c r="G79" s="42">
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2848,13 +2784,12 @@
       <c r="E80" s="28">
         <v>0.53589120370370369</v>
       </c>
-      <c r="F80" s="37">
-        <f t="shared" si="2"/>
+      <c r="F80" s="36">
+        <f t="shared" si="1"/>
         <v>6.018518518517979E-4</v>
       </c>
-      <c r="G80" s="38">
-        <f t="shared" si="3"/>
-        <v>6.018518518517979E-4</v>
+      <c r="G80" s="42">
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2873,13 +2808,12 @@
       <c r="E81" s="28">
         <v>0.53686342592592595</v>
       </c>
-      <c r="F81" s="37">
-        <f t="shared" si="2"/>
+      <c r="F81" s="36">
+        <f t="shared" si="1"/>
         <v>7.4074074074081953E-4</v>
       </c>
-      <c r="G81" s="38">
-        <f t="shared" si="3"/>
-        <v>7.4074074074081953E-4</v>
+      <c r="G81" s="42">
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2898,13 +2832,12 @@
       <c r="E82" s="28">
         <v>0.53738425925925926</v>
       </c>
-      <c r="F82" s="37">
-        <f t="shared" si="2"/>
+      <c r="F82" s="36">
+        <f t="shared" si="1"/>
         <v>3.8194444444450415E-4</v>
       </c>
-      <c r="G82" s="38">
-        <f t="shared" si="3"/>
-        <v>3.8194444444450415E-4</v>
+      <c r="G82" s="42">
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2923,13 +2856,12 @@
       <c r="E83" s="28">
         <v>0.53789351851851852</v>
       </c>
-      <c r="F83" s="37">
-        <f t="shared" si="2"/>
+      <c r="F83" s="36">
+        <f t="shared" si="1"/>
         <v>4.8611111111107608E-4</v>
       </c>
-      <c r="G83" s="38">
-        <f t="shared" si="3"/>
-        <v>4.8611111111107608E-4</v>
+      <c r="G83" s="42">
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2948,13 +2880,12 @@
       <c r="E84" s="28">
         <v>0.5385416666666667</v>
       </c>
-      <c r="F84" s="37">
-        <f t="shared" si="2"/>
+      <c r="F84" s="36">
+        <f t="shared" si="1"/>
         <v>6.3657407407413658E-4</v>
       </c>
-      <c r="G84" s="38">
-        <f t="shared" si="3"/>
-        <v>6.3657407407413658E-4</v>
+      <c r="G84" s="42">
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2973,13 +2904,12 @@
       <c r="E85" s="28">
         <v>0.53965277777777776</v>
       </c>
-      <c r="F85" s="37">
-        <f t="shared" si="2"/>
+      <c r="F85" s="36">
+        <f t="shared" si="1"/>
         <v>1.0763888888888351E-3</v>
       </c>
-      <c r="G85" s="38">
-        <f t="shared" si="3"/>
-        <v>1.0763888888888351E-3</v>
+      <c r="G85" s="42">
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2998,13 +2928,12 @@
       <c r="E86" s="28">
         <v>0.54010416666666672</v>
       </c>
-      <c r="F86" s="37">
-        <f t="shared" si="2"/>
+      <c r="F86" s="36">
+        <f t="shared" si="1"/>
         <v>4.0509259259269292E-4</v>
       </c>
-      <c r="G86" s="38">
-        <f t="shared" si="3"/>
-        <v>4.0509259259269292E-4</v>
+      <c r="G86" s="42">
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3023,13 +2952,12 @@
       <c r="E87" s="28">
         <v>0.54094907407407411</v>
       </c>
-      <c r="F87" s="37">
-        <f t="shared" si="2"/>
+      <c r="F87" s="36">
+        <f t="shared" si="1"/>
         <v>7.9861111111112493E-4</v>
       </c>
-      <c r="G87" s="38">
-        <f t="shared" si="3"/>
-        <v>7.9861111111112493E-4</v>
+      <c r="G87" s="42">
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3048,13 +2976,12 @@
       <c r="E88" s="28">
         <v>0.54126157407407405</v>
       </c>
-      <c r="F88" s="37">
-        <f t="shared" si="2"/>
+      <c r="F88" s="36">
+        <f t="shared" si="1"/>
         <v>1.3888888888879958E-4</v>
       </c>
-      <c r="G88" s="38">
-        <f t="shared" si="3"/>
-        <v>1.3888888888879958E-4</v>
+      <c r="G88" s="42">
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3073,13 +3000,12 @@
       <c r="E89" s="28">
         <v>0.54199074074074072</v>
       </c>
-      <c r="F89" s="37">
-        <f t="shared" si="2"/>
+      <c r="F89" s="36">
+        <f t="shared" si="1"/>
         <v>6.2499999999998668E-4</v>
       </c>
-      <c r="G89" s="38">
-        <f t="shared" si="3"/>
-        <v>6.2499999999998668E-4</v>
+      <c r="G89" s="42">
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3098,13 +3024,12 @@
       <c r="E90" s="28">
         <v>0.54259259259259263</v>
       </c>
-      <c r="F90" s="37">
-        <f t="shared" si="2"/>
+      <c r="F90" s="36">
+        <f t="shared" si="1"/>
         <v>5.7870370370372015E-4</v>
       </c>
-      <c r="G90" s="38">
-        <f t="shared" si="3"/>
-        <v>5.7870370370372015E-4</v>
+      <c r="G90" s="42">
+        <v>50</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3123,13 +3048,12 @@
       <c r="E91" s="28">
         <v>0.54309027777777774</v>
       </c>
-      <c r="F91" s="37">
-        <f t="shared" si="2"/>
+      <c r="F91" s="36">
+        <f t="shared" si="1"/>
         <v>1.7361111111113825E-4</v>
       </c>
-      <c r="G91" s="38">
-        <f t="shared" si="3"/>
-        <v>1.7361111111113825E-4</v>
+      <c r="G91" s="42">
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3148,13 +3072,12 @@
       <c r="E92" s="28">
         <v>0.54402777777777778</v>
       </c>
-      <c r="F92" s="37">
-        <f t="shared" si="2"/>
+      <c r="F92" s="36">
+        <f t="shared" si="1"/>
         <v>9.0277777777780788E-4</v>
       </c>
-      <c r="G92" s="38">
-        <f t="shared" si="3"/>
-        <v>9.0277777777780788E-4</v>
+      <c r="G92" s="42">
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3173,13 +3096,12 @@
       <c r="E93" s="28">
         <v>0.54452546296296289</v>
       </c>
-      <c r="F93" s="37">
-        <f t="shared" si="2"/>
+      <c r="F93" s="36">
+        <f t="shared" si="1"/>
         <v>4.7453703703692618E-4</v>
       </c>
-      <c r="G93" s="38">
-        <f t="shared" si="3"/>
-        <v>4.7453703703692618E-4</v>
+      <c r="G93" s="42">
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3198,13 +3120,12 @@
       <c r="E94" s="28">
         <v>0.54533564814814817</v>
       </c>
-      <c r="F94" s="37">
-        <f t="shared" si="2"/>
+      <c r="F94" s="36">
+        <f t="shared" si="1"/>
         <v>7.8703703703708605E-4</v>
       </c>
-      <c r="G94" s="38">
-        <f t="shared" si="3"/>
-        <v>7.8703703703708605E-4</v>
+      <c r="G94" s="42">
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3223,13 +3144,12 @@
       <c r="E95" s="28">
         <v>0.54579861111111116</v>
       </c>
-      <c r="F95" s="37">
-        <f t="shared" si="2"/>
+      <c r="F95" s="36">
+        <f t="shared" si="1"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="G95" s="38">
-        <f t="shared" si="3"/>
-        <v>4.3981481481480955E-4</v>
+      <c r="G95" s="42">
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3248,13 +3168,12 @@
       <c r="E96" s="28">
         <v>0.54615740740740748</v>
       </c>
-      <c r="F96" s="37">
-        <f t="shared" si="2"/>
+      <c r="F96" s="36">
+        <f t="shared" si="1"/>
         <v>3.5879629629631538E-4</v>
       </c>
-      <c r="G96" s="38">
-        <f t="shared" si="3"/>
-        <v>3.5879629629631538E-4</v>
+      <c r="G96" s="42">
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3273,13 +3192,12 @@
       <c r="E97" s="28">
         <v>0.54638888888888892</v>
       </c>
-      <c r="F97" s="37">
-        <f t="shared" si="2"/>
+      <c r="F97" s="36">
+        <f t="shared" si="1"/>
         <v>1.9675925925932702E-4</v>
       </c>
-      <c r="G97" s="38">
-        <f t="shared" si="3"/>
-        <v>1.9675925925932702E-4</v>
+      <c r="G97" s="42">
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3298,13 +3216,12 @@
       <c r="E98" s="28">
         <v>0.54673611111111109</v>
       </c>
-      <c r="F98" s="37">
-        <f t="shared" si="2"/>
+      <c r="F98" s="36">
+        <f t="shared" si="1"/>
         <v>3.356481481481266E-4</v>
       </c>
-      <c r="G98" s="38">
-        <f t="shared" si="3"/>
-        <v>3.356481481481266E-4</v>
+      <c r="G98" s="42">
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3323,13 +3240,12 @@
       <c r="E99" s="28">
         <v>0.54700231481481476</v>
       </c>
-      <c r="F99" s="37">
-        <f t="shared" si="2"/>
+      <c r="F99" s="36">
+        <f t="shared" si="1"/>
         <v>2.546296296295214E-4</v>
       </c>
-      <c r="G99" s="38">
-        <f t="shared" si="3"/>
-        <v>2.546296296295214E-4</v>
+      <c r="G99" s="42">
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3348,13 +3264,12 @@
       <c r="E100" s="28">
         <v>0.54723379629629632</v>
       </c>
-      <c r="F100" s="37">
-        <f t="shared" si="2"/>
+      <c r="F100" s="36">
+        <f t="shared" si="1"/>
         <v>2.1990740740740478E-4</v>
       </c>
-      <c r="G100" s="38">
-        <f t="shared" si="3"/>
-        <v>2.1990740740740478E-4</v>
+      <c r="G100" s="42">
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3373,13 +3288,12 @@
       <c r="E101" s="28">
         <v>0.54775462962962962</v>
       </c>
-      <c r="F101" s="37">
-        <f t="shared" si="2"/>
+      <c r="F101" s="36">
+        <f t="shared" si="1"/>
         <v>3.356481481481266E-4</v>
       </c>
-      <c r="G101" s="38">
-        <f t="shared" si="3"/>
-        <v>3.356481481481266E-4</v>
+      <c r="G101" s="42">
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3398,13 +3312,12 @@
       <c r="E102" s="28">
         <v>0.54837962962962961</v>
       </c>
-      <c r="F102" s="37">
-        <f t="shared" si="2"/>
+      <c r="F102" s="36">
+        <f t="shared" si="1"/>
         <v>6.2499999999998668E-4</v>
       </c>
-      <c r="G102" s="38">
-        <f t="shared" si="3"/>
-        <v>6.2499999999998668E-4</v>
+      <c r="G102" s="42">
+        <v>54</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3415,12 +3328,11 @@
       <c r="C103" s="28"/>
       <c r="D103" s="35"/>
       <c r="E103" s="28"/>
-      <c r="F103" s="37">
-        <f t="shared" si="2"/>
+      <c r="F103" s="36">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G103" s="38">
-        <f t="shared" si="3"/>
+      <c r="G103" s="42">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data pripravene na analyzu
</commit_message>
<xml_diff>
--- a/data-supermarket.xlsx
+++ b/data-supermarket.xlsx
@@ -17,10 +17,14 @@
     <sheet name="Kým sa pozbiera z pohladne" sheetId="2" r:id="rId3"/>
     <sheet name="Čas v systéme" sheetId="4" r:id="rId4"/>
     <sheet name="Veľkosť radu pri pokladni" sheetId="5" r:id="rId5"/>
+    <sheet name="Rozdiely príchodov" sheetId="6" r:id="rId6"/>
+    <sheet name="Počet ludí v príchod" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="doba_obsluhypokladne_1" localSheetId="0">'Obsluha na pokladni'!$B$4:$E$102</definedName>
-    <definedName name="New_Text_Document" localSheetId="0">'Obsluha na pokladni'!$G$4:$G$103</definedName>
+    <definedName name="doba_obsluhypokladne_1" localSheetId="0">'Obsluha na pokladni'!$B$4:$E$101</definedName>
+    <definedName name="New_Text_Document" localSheetId="0">'Obsluha na pokladni'!$G$4:$G$102</definedName>
+    <definedName name="pocet_prichLudi" localSheetId="6">'Počet ludí v príchod'!$A$1:$B$39</definedName>
+    <definedName name="pocet_prichLudi_1" localSheetId="5">'Rozdiely príchodov'!$A$1:$B$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -50,11 +54,27 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="pocet_prichLudi" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\pocet_prichLudi.txt" tab="0" space="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="pocet_prichLudi1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\pocet_prichLudi.txt" space="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Por. Číslo</t>
   </si>
@@ -160,6 +180,30 @@
   <si>
     <t>Doba obsluhy na pokladni</t>
   </si>
+  <si>
+    <t>Pocet udajov</t>
+  </si>
+  <si>
+    <t>Veľkosť skupiny</t>
+  </si>
+  <si>
+    <t>Počet výskytov</t>
+  </si>
+  <si>
+    <t>Percentá</t>
+  </si>
+  <si>
+    <t>Spolu</t>
+  </si>
+  <si>
+    <t>Cas odchodu z pokladne</t>
+  </si>
+  <si>
+    <t>Sekundy</t>
+  </si>
+  <si>
+    <t>pocet</t>
+  </si>
 </sst>
 </file>
 
@@ -254,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -417,11 +461,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,10 +560,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,11 +595,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,31 +884,32 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="9" max="10" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
@@ -859,8 +931,14 @@
       <c r="G3" s="37" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -880,15 +958,28 @@
         <f>E4-C4</f>
         <v>5.4398148148154801E-4</v>
       </c>
-      <c r="G4" s="42">
-        <v>47</v>
+      <c r="G4" s="41">
+        <f>F4*86400</f>
+        <v>47.000000000005748</v>
+      </c>
+      <c r="H4" t="e">
+        <f>se</f>
+        <v>#NAME?</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="45">
+        <f>C5-E4</f>
+        <v>3.4722222222172139E-5</v>
+      </c>
+      <c r="M4" s="43">
+        <f>L4*86400</f>
+        <v>2.9999999999956728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>2</v>
       </c>
@@ -908,13 +999,22 @@
         <f t="shared" ref="F5:F68" si="0">E5-C5</f>
         <v>1.1458333333333459E-3</v>
       </c>
-      <c r="G5" s="42">
-        <v>99</v>
+      <c r="G5" s="41">
+        <f t="shared" ref="G5:G68" si="1">F5*86400</f>
+        <v>99.00000000000108</v>
       </c>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="45">
+        <f t="shared" ref="L5:L68" si="2">C6-E5</f>
+        <v>2.3148148148133263E-5</v>
+      </c>
+      <c r="M5" s="43">
+        <f t="shared" ref="M5:M68" si="3">L5*86400</f>
+        <v>1.9999999999987139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>3</v>
       </c>
@@ -934,8 +1034,9 @@
         <f t="shared" si="0"/>
         <v>1.8518518518523264E-4</v>
       </c>
-      <c r="G6" s="42">
-        <v>16</v>
+      <c r="G6" s="41">
+        <f t="shared" si="1"/>
+        <v>16.0000000000041</v>
       </c>
       <c r="I6" s="38" t="s">
         <v>21</v>
@@ -943,8 +1044,16 @@
       <c r="J6" s="38">
         <v>43.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222172139E-5</v>
+      </c>
+      <c r="M6" s="43">
+        <f t="shared" si="3"/>
+        <v>2.9999999999956728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>4</v>
       </c>
@@ -964,8 +1073,9 @@
         <f t="shared" si="0"/>
         <v>2.777777777778212E-4</v>
       </c>
-      <c r="G7" s="42">
-        <v>24</v>
+      <c r="G7" s="41">
+        <f t="shared" si="1"/>
+        <v>24.000000000003752</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>22</v>
@@ -973,8 +1083,16 @@
       <c r="J7" s="38">
         <v>2.4038689354009835</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="45">
+        <f t="shared" si="2"/>
+        <v>4.6296296296266526E-5</v>
+      </c>
+      <c r="M7" s="43">
+        <f t="shared" si="3"/>
+        <v>3.9999999999974278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>5</v>
       </c>
@@ -994,8 +1112,9 @@
         <f t="shared" si="0"/>
         <v>9.6064814814816879E-4</v>
       </c>
-      <c r="G8" s="42">
-        <v>83</v>
+      <c r="G8" s="41">
+        <f t="shared" si="1"/>
+        <v>83.000000000001791</v>
       </c>
       <c r="I8" s="38" t="s">
         <v>23</v>
@@ -1003,8 +1122,16 @@
       <c r="J8" s="38">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="45">
+        <f t="shared" si="2"/>
+        <v>9.2592592592588563E-5</v>
+      </c>
+      <c r="M8" s="43">
+        <f t="shared" si="3"/>
+        <v>7.9999999999996518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>6</v>
       </c>
@@ -1024,8 +1151,9 @@
         <f t="shared" si="0"/>
         <v>5.7870370370360913E-5</v>
       </c>
-      <c r="G9" s="42">
-        <v>5</v>
+      <c r="G9" s="41">
+        <f t="shared" si="1"/>
+        <v>4.9999999999991829</v>
       </c>
       <c r="I9" s="38" t="s">
         <v>24</v>
@@ -1033,8 +1161,16 @@
       <c r="J9" s="38">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222283161E-5</v>
+      </c>
+      <c r="M9" s="43">
+        <f t="shared" si="3"/>
+        <v>3.0000000000052651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>7</v>
       </c>
@@ -1054,8 +1190,9 @@
         <f t="shared" si="0"/>
         <v>3.3564814814807109E-4</v>
       </c>
-      <c r="G10" s="42">
-        <v>29</v>
+      <c r="G10" s="41">
+        <f t="shared" si="1"/>
+        <v>28.999999999993342</v>
       </c>
       <c r="I10" s="38" t="s">
         <v>25</v>
@@ -1063,8 +1200,16 @@
       <c r="J10" s="38">
         <v>24.038689354009836</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="45">
+        <f t="shared" si="2"/>
+        <v>8.1018518518549687E-5</v>
+      </c>
+      <c r="M10" s="43">
+        <f t="shared" si="3"/>
+        <v>7.000000000002693</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>8</v>
       </c>
@@ -1084,8 +1229,9 @@
         <f t="shared" si="0"/>
         <v>2.3148148148144365E-4</v>
       </c>
-      <c r="G11" s="42">
-        <v>20</v>
+      <c r="G11" s="41">
+        <f t="shared" si="1"/>
+        <v>19.999999999996732</v>
       </c>
       <c r="I11" s="38" t="s">
         <v>26</v>
@@ -1093,8 +1239,16 @@
       <c r="J11" s="38">
         <v>577.85858585858591</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="45">
+        <f t="shared" si="2"/>
+        <v>1.388888888889106E-4</v>
+      </c>
+      <c r="M11" s="43">
+        <f t="shared" si="3"/>
+        <v>12.000000000001876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>9</v>
       </c>
@@ -1114,8 +1268,9 @@
         <f t="shared" si="0"/>
         <v>4.0509259259263741E-4</v>
       </c>
-      <c r="G12" s="42">
-        <v>35</v>
+      <c r="G12" s="41">
+        <f t="shared" si="1"/>
+        <v>35.000000000003872</v>
       </c>
       <c r="I12" s="38" t="s">
         <v>27</v>
@@ -1123,8 +1278,16 @@
       <c r="J12" s="38">
         <v>2.4605882226919138</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="45">
+        <f t="shared" si="2"/>
+        <v>1.7361111111108274E-4</v>
+      </c>
+      <c r="M12" s="43">
+        <f t="shared" si="3"/>
+        <v>14.999999999997549</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>10</v>
       </c>
@@ -1144,8 +1307,9 @@
         <f t="shared" si="0"/>
         <v>3.0092592592589895E-4</v>
       </c>
-      <c r="G13" s="42">
-        <v>26</v>
+      <c r="G13" s="41">
+        <f t="shared" si="1"/>
+        <v>25.999999999997669</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>28</v>
@@ -1153,8 +1317,16 @@
       <c r="J13" s="38">
         <v>1.0425245334884037</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" s="45">
+        <f t="shared" si="2"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="M13" s="43">
+        <f t="shared" si="3"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>11</v>
       </c>
@@ -1174,8 +1346,9 @@
         <f t="shared" si="0"/>
         <v>1.6898148148148384E-3</v>
       </c>
-      <c r="G14" s="42">
-        <v>146</v>
+      <c r="G14" s="41">
+        <f t="shared" si="1"/>
+        <v>146.00000000000205</v>
       </c>
       <c r="I14" s="38" t="s">
         <v>29</v>
@@ -1183,8 +1356,16 @@
       <c r="J14" s="38">
         <v>146</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222222099E-4</v>
+      </c>
+      <c r="M14" s="43">
+        <f t="shared" si="3"/>
+        <v>29.999999999999893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>12</v>
       </c>
@@ -1204,8 +1385,9 @@
         <f t="shared" si="0"/>
         <v>2.8935185185186008E-4</v>
       </c>
-      <c r="G15" s="42">
-        <v>25</v>
+      <c r="G15" s="41">
+        <f t="shared" si="1"/>
+        <v>25.000000000000711</v>
       </c>
       <c r="I15" s="38" t="s">
         <v>30</v>
@@ -1213,8 +1395,16 @@
       <c r="J15" s="38">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370305402E-5</v>
+      </c>
+      <c r="M15" s="43">
+        <f t="shared" si="3"/>
+        <v>4.9999999999943867</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>13</v>
       </c>
@@ -1234,8 +1424,9 @@
         <f t="shared" si="0"/>
         <v>6.9444444444449749E-4</v>
       </c>
-      <c r="G16" s="42">
-        <v>60</v>
+      <c r="G16" s="41">
+        <f t="shared" si="1"/>
+        <v>60.000000000004583</v>
       </c>
       <c r="I16" s="38" t="s">
         <v>31</v>
@@ -1243,8 +1434,16 @@
       <c r="J16" s="38">
         <v>146</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148133263E-5</v>
+      </c>
+      <c r="M16" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999987139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>14</v>
       </c>
@@ -1264,8 +1463,9 @@
         <f t="shared" si="0"/>
         <v>4.0509259259263741E-4</v>
       </c>
-      <c r="G17" s="42">
-        <v>35</v>
+      <c r="G17" s="41">
+        <f t="shared" si="1"/>
+        <v>35.000000000003872</v>
       </c>
       <c r="I17" s="38" t="s">
         <v>32</v>
@@ -1273,8 +1473,16 @@
       <c r="J17" s="38">
         <v>4380</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222172139E-5</v>
+      </c>
+      <c r="M17" s="43">
+        <f t="shared" si="3"/>
+        <v>2.9999999999956728</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27">
         <v>15</v>
       </c>
@@ -1294,8 +1502,9 @@
         <f t="shared" si="0"/>
         <v>3.0092592592589895E-4</v>
       </c>
-      <c r="G18" s="42">
-        <v>26</v>
+      <c r="G18" s="41">
+        <f t="shared" si="1"/>
+        <v>25.999999999997669</v>
       </c>
       <c r="I18" s="39" t="s">
         <v>33</v>
@@ -1303,8 +1512,16 @@
       <c r="J18" s="39">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M18" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>16</v>
       </c>
@@ -1324,11 +1541,20 @@
         <f t="shared" si="0"/>
         <v>3.5879629629631538E-4</v>
       </c>
-      <c r="G19" s="42">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="41">
+        <f t="shared" si="1"/>
+        <v>31.000000000001648</v>
+      </c>
+      <c r="L19" s="45">
+        <f t="shared" si="2"/>
+        <v>7.1759259259251973E-4</v>
+      </c>
+      <c r="M19" s="43">
+        <f t="shared" si="3"/>
+        <v>61.999999999993705</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>17</v>
       </c>
@@ -1348,11 +1574,20 @@
         <f t="shared" si="0"/>
         <v>3.3564814814818211E-4</v>
       </c>
-      <c r="G20" s="42">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="41">
+        <f t="shared" si="1"/>
+        <v>29.000000000002935</v>
+      </c>
+      <c r="L20" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148133263E-5</v>
+      </c>
+      <c r="M20" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999987139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>18</v>
       </c>
@@ -1372,11 +1607,20 @@
         <f t="shared" si="0"/>
         <v>8.4490740740739145E-4</v>
       </c>
-      <c r="G21" s="42">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="41">
+        <f t="shared" si="1"/>
+        <v>72.999999999998622</v>
+      </c>
+      <c r="L21" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074094387E-5</v>
+      </c>
+      <c r="M21" s="43">
+        <f t="shared" si="3"/>
+        <v>1.000000000001755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>19</v>
       </c>
@@ -1396,11 +1640,20 @@
         <f t="shared" si="0"/>
         <v>7.5231481481480289E-4</v>
       </c>
-      <c r="G22" s="42">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="41">
+        <f t="shared" si="1"/>
+        <v>64.999999999998977</v>
+      </c>
+      <c r="L22" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M22" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>20</v>
       </c>
@@ -1420,11 +1673,20 @@
         <f t="shared" si="0"/>
         <v>5.6712962962962576E-4</v>
       </c>
-      <c r="G23" s="42">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G23" s="41">
+        <f t="shared" si="1"/>
+        <v>48.999999999999666</v>
+      </c>
+      <c r="L23" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148077752E-5</v>
+      </c>
+      <c r="M23" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999939178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>21</v>
       </c>
@@ -1444,11 +1706,20 @@
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G24" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="41">
+        <f t="shared" si="1"/>
+        <v>42.000000000006565</v>
+      </c>
+      <c r="L24" s="45">
+        <f t="shared" si="2"/>
+        <v>4.3981481481480955E-4</v>
+      </c>
+      <c r="M24" s="43">
+        <f t="shared" si="3"/>
+        <v>37.999999999999545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>22</v>
       </c>
@@ -1468,11 +1739,20 @@
         <f t="shared" si="0"/>
         <v>6.8287037037029208E-4</v>
       </c>
-      <c r="G25" s="42">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="41">
+        <f t="shared" si="1"/>
+        <v>58.999999999993236</v>
+      </c>
+      <c r="L25" s="45">
+        <f t="shared" si="2"/>
+        <v>1.6203703703709937E-4</v>
+      </c>
+      <c r="M25" s="43">
+        <f t="shared" si="3"/>
+        <v>14.000000000005386</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>23</v>
       </c>
@@ -1492,11 +1772,20 @@
         <f t="shared" si="0"/>
         <v>1.0185185185185297E-3</v>
       </c>
-      <c r="G26" s="42">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="41">
+        <f t="shared" si="1"/>
+        <v>88.000000000000966</v>
+      </c>
+      <c r="L26" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M26" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>24</v>
       </c>
@@ -1516,11 +1805,20 @@
         <f t="shared" si="0"/>
         <v>4.7453703703692618E-4</v>
       </c>
-      <c r="G27" s="42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="41">
+        <f t="shared" si="1"/>
+        <v>40.999999999990422</v>
+      </c>
+      <c r="L27" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M27" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>25</v>
       </c>
@@ -1540,11 +1838,20 @@
         <f t="shared" si="0"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="G28" s="42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="41">
+        <f t="shared" si="1"/>
+        <v>37.999999999999545</v>
+      </c>
+      <c r="L28" s="45">
+        <f t="shared" si="2"/>
+        <v>4.6296296296266526E-5</v>
+      </c>
+      <c r="M28" s="43">
+        <f t="shared" si="3"/>
+        <v>3.9999999999974278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>26</v>
       </c>
@@ -1564,11 +1871,20 @@
         <f t="shared" si="0"/>
         <v>5.7870370370372015E-4</v>
       </c>
-      <c r="G29" s="42">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29" s="41">
+        <f t="shared" si="1"/>
+        <v>50.000000000001421</v>
+      </c>
+      <c r="L29" s="45">
+        <f t="shared" si="2"/>
+        <v>4.6296296296377548E-5</v>
+      </c>
+      <c r="M29" s="43">
+        <f t="shared" si="3"/>
+        <v>4.0000000000070202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>27</v>
       </c>
@@ -1588,11 +1904,20 @@
         <f t="shared" si="0"/>
         <v>3.4722222222216548E-4</v>
       </c>
-      <c r="G30" s="42">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="41">
+        <f t="shared" si="1"/>
+        <v>29.999999999995097</v>
+      </c>
+      <c r="L30" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M30" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>28</v>
       </c>
@@ -1612,11 +1937,20 @@
         <f t="shared" si="0"/>
         <v>6.5972222222221433E-4</v>
       </c>
-      <c r="G31" s="42">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="41">
+        <f t="shared" si="1"/>
+        <v>56.999999999999318</v>
+      </c>
+      <c r="L31" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222116628E-5</v>
+      </c>
+      <c r="M31" s="43">
+        <f t="shared" si="3"/>
+        <v>2.9999999999908766</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <v>29</v>
       </c>
@@ -1636,11 +1970,20 @@
         <f t="shared" si="0"/>
         <v>2.5462962962974345E-4</v>
       </c>
-      <c r="G32" s="42">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="41">
+        <f t="shared" si="1"/>
+        <v>22.000000000009834</v>
+      </c>
+      <c r="L32" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148077752E-5</v>
+      </c>
+      <c r="M32" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999939178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <v>30</v>
       </c>
@@ -1660,11 +2003,20 @@
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G33" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="41">
+        <f t="shared" si="1"/>
+        <v>42.000000000006565</v>
+      </c>
+      <c r="L33" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M33" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
         <v>31</v>
       </c>
@@ -1684,11 +2036,20 @@
         <f t="shared" si="0"/>
         <v>6.018518518517979E-4</v>
       </c>
-      <c r="G34" s="42">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="41">
+        <f t="shared" si="1"/>
+        <v>51.999999999995339</v>
+      </c>
+      <c r="L34" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370416424E-5</v>
+      </c>
+      <c r="M34" s="43">
+        <f t="shared" si="3"/>
+        <v>5.000000000003979</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <v>32</v>
       </c>
@@ -1708,11 +2069,20 @@
         <f t="shared" si="0"/>
         <v>3.1249999999993783E-4</v>
       </c>
-      <c r="G35" s="42">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="41">
+        <f t="shared" si="1"/>
+        <v>26.999999999994628</v>
+      </c>
+      <c r="L35" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M35" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
         <v>33</v>
       </c>
@@ -1732,11 +2102,20 @@
         <f t="shared" si="0"/>
         <v>6.9444444444444198E-4</v>
       </c>
-      <c r="G36" s="42">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="41">
+        <f t="shared" si="1"/>
+        <v>59.999999999999787</v>
+      </c>
+      <c r="L36" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148077752E-5</v>
+      </c>
+      <c r="M36" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999939178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>34</v>
       </c>
@@ -1756,11 +2135,20 @@
         <f t="shared" si="0"/>
         <v>3.8194444444450415E-4</v>
       </c>
-      <c r="G37" s="42">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="41">
+        <f t="shared" si="1"/>
+        <v>33.000000000005159</v>
+      </c>
+      <c r="L37" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M37" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>35</v>
       </c>
@@ -1780,11 +2168,20 @@
         <f t="shared" si="0"/>
         <v>4.6296296296299833E-4</v>
       </c>
-      <c r="G38" s="42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="41">
+        <f t="shared" si="1"/>
+        <v>40.000000000003055</v>
+      </c>
+      <c r="L38" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M38" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <v>36</v>
       </c>
@@ -1804,11 +2201,20 @@
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G39" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="41">
+        <f t="shared" si="1"/>
+        <v>42.000000000006565</v>
+      </c>
+      <c r="L39" s="45">
+        <f t="shared" si="2"/>
+        <v>8.1018518518494176E-5</v>
+      </c>
+      <c r="M39" s="43">
+        <f t="shared" si="3"/>
+        <v>6.9999999999978968</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <v>37</v>
       </c>
@@ -1828,11 +2234,20 @@
         <f t="shared" si="0"/>
         <v>1.1574074074074403E-3</v>
       </c>
-      <c r="G40" s="42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="41">
+        <f t="shared" si="1"/>
+        <v>100.00000000000284</v>
+      </c>
+      <c r="L40" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074072183E-4</v>
+      </c>
+      <c r="M40" s="43">
+        <f t="shared" si="3"/>
+        <v>9.9999999999983658</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <v>38</v>
       </c>
@@ -1852,11 +2267,20 @@
         <f t="shared" si="0"/>
         <v>2.0833333333325488E-4</v>
       </c>
-      <c r="G41" s="42">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="41">
+        <f t="shared" si="1"/>
+        <v>17.999999999993221</v>
+      </c>
+      <c r="L41" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M41" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <v>39</v>
       </c>
@@ -1876,11 +2300,20 @@
         <f t="shared" si="0"/>
         <v>6.018518518517979E-4</v>
       </c>
-      <c r="G42" s="42">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="41">
+        <f t="shared" si="1"/>
+        <v>51.999999999995339</v>
+      </c>
+      <c r="L42" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M42" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <v>40</v>
       </c>
@@ -1900,11 +2333,20 @@
         <f t="shared" si="0"/>
         <v>8.1018518518494176E-5</v>
       </c>
-      <c r="G43" s="42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="41">
+        <f t="shared" si="1"/>
+        <v>6.9999999999978968</v>
+      </c>
+      <c r="L43" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M43" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <v>41</v>
       </c>
@@ -1924,11 +2366,20 @@
         <f t="shared" si="0"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="G44" s="42">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="41">
+        <f t="shared" si="1"/>
+        <v>44.000000000000483</v>
+      </c>
+      <c r="L44" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M44" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <v>42</v>
       </c>
@@ -1948,11 +2399,20 @@
         <f t="shared" si="0"/>
         <v>6.134259259259478E-4</v>
       </c>
-      <c r="G45" s="42">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="41">
+        <f t="shared" si="1"/>
+        <v>53.00000000000189</v>
+      </c>
+      <c r="L45" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370416424E-5</v>
+      </c>
+      <c r="M45" s="43">
+        <f t="shared" si="3"/>
+        <v>5.000000000003979</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <v>43</v>
       </c>
@@ -1972,11 +2432,20 @@
         <f t="shared" si="0"/>
         <v>5.324074074073426E-4</v>
       </c>
-      <c r="G46" s="42">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="41">
+        <f t="shared" si="1"/>
+        <v>45.999999999994401</v>
+      </c>
+      <c r="L46" s="45">
+        <f t="shared" si="2"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="M46" s="43">
+        <f t="shared" si="3"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <v>44</v>
       </c>
@@ -1996,11 +2465,20 @@
         <f t="shared" si="0"/>
         <v>8.4490740740750248E-4</v>
       </c>
-      <c r="G47" s="42">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="41">
+        <f t="shared" si="1"/>
+        <v>73.000000000008214</v>
+      </c>
+      <c r="L47" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M47" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
         <v>45</v>
       </c>
@@ -2020,11 +2498,20 @@
         <f t="shared" si="0"/>
         <v>6.712962962962532E-4</v>
       </c>
-      <c r="G48" s="42">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="41">
+        <f t="shared" si="1"/>
+        <v>57.999999999996277</v>
+      </c>
+      <c r="L48" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M48" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <v>46</v>
       </c>
@@ -2044,11 +2531,20 @@
         <f t="shared" si="0"/>
         <v>2.7777777777771018E-4</v>
       </c>
-      <c r="G49" s="42">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="41">
+        <f t="shared" si="1"/>
+        <v>23.999999999994159</v>
+      </c>
+      <c r="L49" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M49" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <v>47</v>
       </c>
@@ -2068,11 +2564,20 @@
         <f t="shared" si="0"/>
         <v>1.388888888889106E-4</v>
       </c>
-      <c r="G50" s="42">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="41">
+        <f t="shared" si="1"/>
+        <v>12.000000000001876</v>
+      </c>
+      <c r="L50" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M50" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <v>48</v>
       </c>
@@ -2092,11 +2597,20 @@
         <f t="shared" si="0"/>
         <v>2.4305555555559355E-4</v>
       </c>
-      <c r="G51" s="42">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="41">
+        <f t="shared" si="1"/>
+        <v>21.000000000003283</v>
+      </c>
+      <c r="L51" s="45">
+        <f t="shared" si="2"/>
+        <v>3.4722222222116628E-5</v>
+      </c>
+      <c r="M51" s="43">
+        <f t="shared" si="3"/>
+        <v>2.9999999999908766</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
         <v>49</v>
       </c>
@@ -2116,11 +2630,20 @@
         <f t="shared" si="0"/>
         <v>1.7361111111113825E-4</v>
       </c>
-      <c r="G52" s="42">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="41">
+        <f t="shared" si="1"/>
+        <v>15.000000000002345</v>
+      </c>
+      <c r="L52" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M52" s="43">
+        <f t="shared" si="3"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
         <v>50</v>
       </c>
@@ -2140,11 +2663,20 @@
         <f t="shared" si="0"/>
         <v>8.3333333333324155E-4</v>
       </c>
-      <c r="G53" s="42">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="41">
+        <f t="shared" si="1"/>
+        <v>71.99999999999207</v>
+      </c>
+      <c r="L53" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M53" s="43">
+        <f t="shared" si="3"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <v>51</v>
       </c>
@@ -2164,11 +2696,20 @@
         <f t="shared" si="0"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="G54" s="42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="41">
+        <f t="shared" si="1"/>
+        <v>37.999999999999545</v>
+      </c>
+      <c r="L54" s="45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <v>52</v>
       </c>
@@ -2188,11 +2729,20 @@
         <f t="shared" si="0"/>
         <v>4.8611111111107608E-4</v>
       </c>
-      <c r="G55" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="41">
+        <f t="shared" si="1"/>
+        <v>41.999999999996973</v>
+      </c>
+      <c r="L55" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370416424E-5</v>
+      </c>
+      <c r="M55" s="43">
+        <f t="shared" si="3"/>
+        <v>5.000000000003979</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <v>53</v>
       </c>
@@ -2212,11 +2762,20 @@
         <f t="shared" si="0"/>
         <v>7.2916666666666963E-4</v>
       </c>
-      <c r="G56" s="42">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="41">
+        <f t="shared" si="1"/>
+        <v>63.000000000000256</v>
+      </c>
+      <c r="L56" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M56" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <v>54</v>
       </c>
@@ -2236,11 +2795,20 @@
         <f t="shared" si="0"/>
         <v>5.555555555556424E-4</v>
       </c>
-      <c r="G57" s="42">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="41">
+        <f t="shared" si="1"/>
+        <v>48.000000000007503</v>
+      </c>
+      <c r="L57" s="45">
+        <f t="shared" si="2"/>
+        <v>4.6296296296155504E-5</v>
+      </c>
+      <c r="M57" s="43">
+        <f t="shared" si="3"/>
+        <v>3.9999999999878355</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <v>55</v>
       </c>
@@ -2260,11 +2828,20 @@
         <f t="shared" si="0"/>
         <v>3.5879629629631538E-4</v>
       </c>
-      <c r="G58" s="42">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="41">
+        <f t="shared" si="1"/>
+        <v>31.000000000001648</v>
+      </c>
+      <c r="L58" s="45">
+        <f t="shared" si="2"/>
+        <v>4.6296296296377548E-5</v>
+      </c>
+      <c r="M58" s="43">
+        <f t="shared" si="3"/>
+        <v>4.0000000000070202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <v>56</v>
       </c>
@@ -2284,11 +2861,20 @@
         <f t="shared" si="0"/>
         <v>6.3657407407402555E-4</v>
       </c>
-      <c r="G59" s="42">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="41">
+        <f t="shared" si="1"/>
+        <v>54.999999999995808</v>
+      </c>
+      <c r="L59" s="45">
+        <f t="shared" si="2"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="M59" s="43">
+        <f t="shared" si="3"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <v>57</v>
       </c>
@@ -2308,11 +2894,20 @@
         <f t="shared" si="0"/>
         <v>4.2824074074077068E-4</v>
       </c>
-      <c r="G60" s="42">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="41">
+        <f t="shared" si="1"/>
+        <v>37.000000000002586</v>
+      </c>
+      <c r="L60" s="45">
+        <f t="shared" si="2"/>
+        <v>2.3148148148077752E-5</v>
+      </c>
+      <c r="M60" s="43">
+        <f t="shared" si="3"/>
+        <v>1.9999999999939178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <v>58</v>
       </c>
@@ -2332,11 +2927,20 @@
         <f t="shared" si="0"/>
         <v>7.1759259259263075E-4</v>
       </c>
-      <c r="G61" s="42">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="41">
+        <f t="shared" si="1"/>
+        <v>62.000000000003297</v>
+      </c>
+      <c r="L61" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M61" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
         <v>59</v>
       </c>
@@ -2356,11 +2960,20 @@
         <f t="shared" si="0"/>
         <v>5.3240740740745363E-4</v>
       </c>
-      <c r="G62" s="42">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G62" s="41">
+        <f t="shared" si="1"/>
+        <v>46.000000000003993</v>
+      </c>
+      <c r="L62" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370305402E-5</v>
+      </c>
+      <c r="M62" s="43">
+        <f t="shared" si="3"/>
+        <v>4.9999999999943867</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
         <v>60</v>
       </c>
@@ -2380,11 +2993,20 @@
         <f t="shared" si="0"/>
         <v>4.9768518518522598E-4</v>
       </c>
-      <c r="G63" s="42">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="41">
+        <f t="shared" si="1"/>
+        <v>43.000000000003524</v>
+      </c>
+      <c r="L63" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M63" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <v>61</v>
       </c>
@@ -2404,11 +3026,20 @@
         <f t="shared" si="0"/>
         <v>4.861111111111871E-4</v>
       </c>
-      <c r="G64" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="41">
+        <f t="shared" si="1"/>
+        <v>42.000000000006565</v>
+      </c>
+      <c r="L64" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M64" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <v>62</v>
       </c>
@@ -2428,11 +3059,20 @@
         <f t="shared" si="0"/>
         <v>4.6296296296299833E-4</v>
       </c>
-      <c r="G65" s="42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="41">
+        <f t="shared" si="1"/>
+        <v>40.000000000003055</v>
+      </c>
+      <c r="L65" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M65" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <v>63</v>
       </c>
@@ -2452,11 +3092,20 @@
         <f t="shared" si="0"/>
         <v>5.9027777777787005E-4</v>
       </c>
-      <c r="G66" s="42">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="41">
+        <f t="shared" si="1"/>
+        <v>51.000000000007972</v>
+      </c>
+      <c r="L66" s="45">
+        <f t="shared" si="2"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M66" s="43">
+        <f t="shared" si="3"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <v>64</v>
       </c>
@@ -2476,11 +3125,20 @@
         <f t="shared" si="0"/>
         <v>1.0300925925925686E-3</v>
       </c>
-      <c r="G67" s="42">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="41">
+        <f t="shared" si="1"/>
+        <v>88.999999999997925</v>
+      </c>
+      <c r="L67" s="45">
+        <f t="shared" si="2"/>
+        <v>3.2523148148148051E-3</v>
+      </c>
+      <c r="M67" s="43">
+        <f t="shared" si="3"/>
+        <v>280.99999999999915</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <v>65</v>
       </c>
@@ -2500,11 +3158,20 @@
         <f t="shared" si="0"/>
         <v>8.796296296296191E-4</v>
       </c>
-      <c r="G68" s="42">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="41">
+        <f t="shared" si="1"/>
+        <v>75.999999999999091</v>
+      </c>
+      <c r="L68" s="45">
+        <f t="shared" si="2"/>
+        <v>5.7870370370372015E-4</v>
+      </c>
+      <c r="M68" s="43">
+        <f t="shared" si="3"/>
+        <v>50.000000000001421</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <v>66</v>
       </c>
@@ -2521,14 +3188,23 @@
         <v>0.53020833333333328</v>
       </c>
       <c r="F69" s="36">
-        <f t="shared" ref="F69:F103" si="1">E69-C69</f>
+        <f t="shared" ref="F69:F103" si="4">E69-C69</f>
         <v>3.4722222222216548E-4</v>
       </c>
-      <c r="G69" s="42">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="41">
+        <f t="shared" ref="G69:G103" si="5">F69*86400</f>
+        <v>29.999999999995097</v>
+      </c>
+      <c r="L69" s="45">
+        <f t="shared" ref="L69:L104" si="6">C70-E69</f>
+        <v>4.6296296296377548E-5</v>
+      </c>
+      <c r="M69" s="43">
+        <f t="shared" ref="M69:M102" si="7">L69*86400</f>
+        <v>4.0000000000070202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <v>67</v>
       </c>
@@ -2545,14 +3221,23 @@
         <v>0.53033564814814815</v>
       </c>
       <c r="F70" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.1018518518494176E-5</v>
       </c>
-      <c r="G70" s="42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="41">
+        <f t="shared" si="5"/>
+        <v>6.9999999999978968</v>
+      </c>
+      <c r="L70" s="45">
+        <f t="shared" si="6"/>
+        <v>1.0416666666668295E-4</v>
+      </c>
+      <c r="M70" s="43">
+        <f t="shared" si="7"/>
+        <v>9.0000000000014069</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <v>68</v>
       </c>
@@ -2560,23 +3245,32 @@
         <v>42684</v>
       </c>
       <c r="C71" s="28">
-        <v>0.53038194444444442</v>
+        <v>0.53043981481481484</v>
       </c>
       <c r="D71" s="35">
         <v>42684</v>
       </c>
       <c r="E71" s="28">
-        <v>0.53039351851851857</v>
+        <v>0.5307291666666667</v>
       </c>
       <c r="F71" s="36">
-        <f t="shared" si="1"/>
-        <v>1.1574074074149898E-5</v>
-      </c>
-      <c r="G71" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.8935185185186008E-4</v>
+      </c>
+      <c r="G71" s="41">
+        <f t="shared" si="5"/>
+        <v>25.000000000000711</v>
+      </c>
+      <c r="L71" s="45">
+        <f t="shared" si="6"/>
+        <v>7.2916666666666963E-4</v>
+      </c>
+      <c r="M71" s="43">
+        <f t="shared" si="7"/>
+        <v>63.000000000000256</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <v>69</v>
       </c>
@@ -2584,23 +3278,32 @@
         <v>42684</v>
       </c>
       <c r="C72" s="28">
-        <v>0.53043981481481484</v>
+        <v>0.53145833333333337</v>
       </c>
       <c r="D72" s="35">
         <v>42684</v>
       </c>
       <c r="E72" s="28">
-        <v>0.5307291666666667</v>
+        <v>0.53234953703703702</v>
       </c>
       <c r="F72" s="36">
-        <f t="shared" si="1"/>
-        <v>2.8935185185186008E-4</v>
-      </c>
-      <c r="G72" s="42">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.9120370370365798E-4</v>
+      </c>
+      <c r="G72" s="41">
+        <f t="shared" si="5"/>
+        <v>76.999999999996049</v>
+      </c>
+      <c r="L72" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M72" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <v>70</v>
       </c>
@@ -2608,23 +3311,32 @@
         <v>42684</v>
       </c>
       <c r="C73" s="28">
-        <v>0.53145833333333337</v>
+        <v>0.53237268518518521</v>
       </c>
       <c r="D73" s="35">
         <v>42684</v>
       </c>
       <c r="E73" s="28">
-        <v>0.53234953703703702</v>
+        <v>0.53288194444444448</v>
       </c>
       <c r="F73" s="36">
-        <f t="shared" si="1"/>
-        <v>8.9120370370365798E-4</v>
-      </c>
-      <c r="G73" s="42">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>5.0925925925926485E-4</v>
+      </c>
+      <c r="G73" s="41">
+        <f t="shared" si="5"/>
+        <v>44.000000000000483</v>
+      </c>
+      <c r="L73" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M73" s="43">
+        <f t="shared" si="7"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <v>71</v>
       </c>
@@ -2632,23 +3344,32 @@
         <v>42684</v>
       </c>
       <c r="C74" s="28">
-        <v>0.53237268518518521</v>
+        <v>0.53289351851851852</v>
       </c>
       <c r="D74" s="35">
         <v>42684</v>
       </c>
       <c r="E74" s="28">
-        <v>0.53288194444444448</v>
+        <v>0.53340277777777778</v>
       </c>
       <c r="F74" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="G74" s="42">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="41">
+        <f t="shared" si="5"/>
+        <v>44.000000000000483</v>
+      </c>
+      <c r="L74" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M74" s="43">
+        <f t="shared" si="7"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <v>72</v>
       </c>
@@ -2656,23 +3377,32 @@
         <v>42684</v>
       </c>
       <c r="C75" s="28">
-        <v>0.53289351851851852</v>
+        <v>0.53341435185185182</v>
       </c>
       <c r="D75" s="35">
         <v>42684</v>
       </c>
       <c r="E75" s="28">
-        <v>0.53340277777777778</v>
+        <v>0.53384259259259259</v>
       </c>
       <c r="F75" s="36">
-        <f t="shared" si="1"/>
-        <v>5.0925925925926485E-4</v>
-      </c>
-      <c r="G75" s="42">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.2824074074077068E-4</v>
+      </c>
+      <c r="G75" s="41">
+        <f t="shared" si="5"/>
+        <v>37.000000000002586</v>
+      </c>
+      <c r="L75" s="45">
+        <f t="shared" si="6"/>
+        <v>4.6296296296266526E-5</v>
+      </c>
+      <c r="M75" s="43">
+        <f t="shared" si="7"/>
+        <v>3.9999999999974278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <v>73</v>
       </c>
@@ -2680,23 +3410,32 @@
         <v>42684</v>
       </c>
       <c r="C76" s="28">
-        <v>0.53341435185185182</v>
+        <v>0.53388888888888886</v>
       </c>
       <c r="D76" s="35">
         <v>42684</v>
       </c>
       <c r="E76" s="28">
-        <v>0.53384259259259259</v>
+        <v>0.53451388888888884</v>
       </c>
       <c r="F76" s="36">
-        <f t="shared" si="1"/>
-        <v>4.2824074074077068E-4</v>
-      </c>
-      <c r="G76" s="42">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.2499999999998668E-4</v>
+      </c>
+      <c r="G76" s="41">
+        <f t="shared" si="5"/>
+        <v>53.999999999998849</v>
+      </c>
+      <c r="L76" s="45">
+        <f t="shared" si="6"/>
+        <v>9.2592592592644074E-5</v>
+      </c>
+      <c r="M76" s="43">
+        <f t="shared" si="7"/>
+        <v>8.000000000004448</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
         <v>74</v>
       </c>
@@ -2704,23 +3443,32 @@
         <v>42684</v>
       </c>
       <c r="C77" s="28">
-        <v>0.53388888888888886</v>
+        <v>0.53460648148148149</v>
       </c>
       <c r="D77" s="35">
         <v>42684</v>
       </c>
       <c r="E77" s="28">
-        <v>0.53451388888888884</v>
+        <v>0.53498842592592599</v>
       </c>
       <c r="F77" s="36">
-        <f t="shared" si="1"/>
-        <v>6.2499999999998668E-4</v>
-      </c>
-      <c r="G77" s="42">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.8194444444450415E-4</v>
+      </c>
+      <c r="G77" s="41">
+        <f t="shared" si="5"/>
+        <v>33.000000000005159</v>
+      </c>
+      <c r="L77" s="45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M77" s="43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
         <v>75</v>
       </c>
@@ -2728,23 +3476,32 @@
         <v>42684</v>
       </c>
       <c r="C78" s="28">
-        <v>0.53460648148148149</v>
+        <v>0.53498842592592599</v>
       </c>
       <c r="D78" s="35">
         <v>42684</v>
       </c>
       <c r="E78" s="28">
-        <v>0.53498842592592599</v>
+        <v>0.5352662037037037</v>
       </c>
       <c r="F78" s="36">
-        <f t="shared" si="1"/>
-        <v>3.8194444444450415E-4</v>
-      </c>
-      <c r="G78" s="42">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.7777777777771018E-4</v>
+      </c>
+      <c r="G78" s="41">
+        <f t="shared" si="5"/>
+        <v>23.999999999994159</v>
+      </c>
+      <c r="L78" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M78" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
         <v>76</v>
       </c>
@@ -2752,23 +3509,32 @@
         <v>42684</v>
       </c>
       <c r="C79" s="28">
-        <v>0.53498842592592599</v>
+        <v>0.53528935185185189</v>
       </c>
       <c r="D79" s="35">
         <v>42684</v>
       </c>
       <c r="E79" s="28">
-        <v>0.5352662037037037</v>
+        <v>0.53589120370370369</v>
       </c>
       <c r="F79" s="36">
-        <f t="shared" si="1"/>
-        <v>2.7777777777771018E-4</v>
-      </c>
-      <c r="G79" s="42">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.018518518517979E-4</v>
+      </c>
+      <c r="G79" s="41">
+        <f t="shared" si="5"/>
+        <v>51.999999999995339</v>
+      </c>
+      <c r="L79" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148144365E-4</v>
+      </c>
+      <c r="M79" s="43">
+        <f t="shared" si="7"/>
+        <v>19.999999999996732</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
         <v>77</v>
       </c>
@@ -2776,23 +3542,32 @@
         <v>42684</v>
       </c>
       <c r="C80" s="28">
-        <v>0.53528935185185189</v>
+        <v>0.53612268518518513</v>
       </c>
       <c r="D80" s="35">
         <v>42684</v>
       </c>
       <c r="E80" s="28">
-        <v>0.53589120370370369</v>
+        <v>0.53686342592592595</v>
       </c>
       <c r="F80" s="36">
-        <f t="shared" si="1"/>
-        <v>6.018518518517979E-4</v>
-      </c>
-      <c r="G80" s="42">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.4074074074081953E-4</v>
+      </c>
+      <c r="G80" s="41">
+        <f t="shared" si="5"/>
+        <v>64.000000000006807</v>
+      </c>
+      <c r="L80" s="45">
+        <f t="shared" si="6"/>
+        <v>1.3888888888879958E-4</v>
+      </c>
+      <c r="M80" s="43">
+        <f t="shared" si="7"/>
+        <v>11.999999999992284</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
         <v>78</v>
       </c>
@@ -2800,23 +3575,32 @@
         <v>42684</v>
       </c>
       <c r="C81" s="28">
-        <v>0.53612268518518513</v>
+        <v>0.53700231481481475</v>
       </c>
       <c r="D81" s="35">
         <v>42684</v>
       </c>
       <c r="E81" s="28">
-        <v>0.53686342592592595</v>
+        <v>0.53738425925925926</v>
       </c>
       <c r="F81" s="36">
-        <f t="shared" si="1"/>
-        <v>7.4074074074081953E-4</v>
-      </c>
-      <c r="G81" s="42">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.8194444444450415E-4</v>
+      </c>
+      <c r="G81" s="41">
+        <f t="shared" si="5"/>
+        <v>33.000000000005159</v>
+      </c>
+      <c r="L81" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M81" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
         <v>79</v>
       </c>
@@ -2824,23 +3608,32 @@
         <v>42684</v>
       </c>
       <c r="C82" s="28">
-        <v>0.53700231481481475</v>
+        <v>0.53740740740740744</v>
       </c>
       <c r="D82" s="35">
         <v>42684</v>
       </c>
       <c r="E82" s="28">
-        <v>0.53738425925925926</v>
+        <v>0.53789351851851852</v>
       </c>
       <c r="F82" s="36">
-        <f t="shared" si="1"/>
-        <v>3.8194444444450415E-4</v>
-      </c>
-      <c r="G82" s="42">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.8611111111107608E-4</v>
+      </c>
+      <c r="G82" s="41">
+        <f t="shared" si="5"/>
+        <v>41.999999999996973</v>
+      </c>
+      <c r="L82" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M82" s="43">
+        <f t="shared" si="7"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
         <v>80</v>
       </c>
@@ -2848,23 +3641,32 @@
         <v>42684</v>
       </c>
       <c r="C83" s="28">
-        <v>0.53740740740740744</v>
+        <v>0.53790509259259256</v>
       </c>
       <c r="D83" s="35">
         <v>42684</v>
       </c>
       <c r="E83" s="28">
-        <v>0.53789351851851852</v>
+        <v>0.5385416666666667</v>
       </c>
       <c r="F83" s="36">
-        <f t="shared" si="1"/>
-        <v>4.8611111111107608E-4</v>
-      </c>
-      <c r="G83" s="42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.3657407407413658E-4</v>
+      </c>
+      <c r="G83" s="41">
+        <f t="shared" si="5"/>
+        <v>55.0000000000054</v>
+      </c>
+      <c r="L83" s="45">
+        <f t="shared" si="6"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="M83" s="43">
+        <f t="shared" si="7"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
         <v>81</v>
       </c>
@@ -2872,23 +3674,32 @@
         <v>42684</v>
       </c>
       <c r="C84" s="28">
-        <v>0.53790509259259256</v>
+        <v>0.53857638888888892</v>
       </c>
       <c r="D84" s="35">
         <v>42684</v>
       </c>
       <c r="E84" s="28">
-        <v>0.5385416666666667</v>
+        <v>0.53965277777777776</v>
       </c>
       <c r="F84" s="36">
-        <f t="shared" si="1"/>
-        <v>6.3657407407413658E-4</v>
-      </c>
-      <c r="G84" s="42">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.0763888888888351E-3</v>
+      </c>
+      <c r="G84" s="41">
+        <f t="shared" si="5"/>
+        <v>92.999999999995353</v>
+      </c>
+      <c r="L84" s="45">
+        <f t="shared" si="6"/>
+        <v>4.6296296296266526E-5</v>
+      </c>
+      <c r="M84" s="43">
+        <f t="shared" si="7"/>
+        <v>3.9999999999974278</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
         <v>82</v>
       </c>
@@ -2896,23 +3707,32 @@
         <v>42684</v>
       </c>
       <c r="C85" s="28">
-        <v>0.53857638888888892</v>
+        <v>0.53969907407407403</v>
       </c>
       <c r="D85" s="35">
         <v>42684</v>
       </c>
       <c r="E85" s="28">
-        <v>0.53965277777777776</v>
+        <v>0.54010416666666672</v>
       </c>
       <c r="F85" s="36">
-        <f t="shared" si="1"/>
-        <v>1.0763888888888351E-3</v>
-      </c>
-      <c r="G85" s="42">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.0509259259269292E-4</v>
+      </c>
+      <c r="G85" s="41">
+        <f t="shared" si="5"/>
+        <v>35.000000000008669</v>
+      </c>
+      <c r="L85" s="45">
+        <f t="shared" si="6"/>
+        <v>4.6296296296266526E-5</v>
+      </c>
+      <c r="M85" s="43">
+        <f t="shared" si="7"/>
+        <v>3.9999999999974278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
         <v>83</v>
       </c>
@@ -2920,23 +3740,32 @@
         <v>42684</v>
       </c>
       <c r="C86" s="28">
-        <v>0.53969907407407403</v>
+        <v>0.54015046296296299</v>
       </c>
       <c r="D86" s="35">
         <v>42684</v>
       </c>
       <c r="E86" s="28">
-        <v>0.54010416666666672</v>
+        <v>0.54094907407407411</v>
       </c>
       <c r="F86" s="36">
-        <f t="shared" si="1"/>
-        <v>4.0509259259269292E-4</v>
-      </c>
-      <c r="G86" s="42">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.9861111111112493E-4</v>
+      </c>
+      <c r="G86" s="41">
+        <f t="shared" si="5"/>
+        <v>69.000000000001194</v>
+      </c>
+      <c r="L86" s="45">
+        <f t="shared" si="6"/>
+        <v>1.7361111111113825E-4</v>
+      </c>
+      <c r="M86" s="43">
+        <f t="shared" si="7"/>
+        <v>15.000000000002345</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
         <v>84</v>
       </c>
@@ -2944,23 +3773,32 @@
         <v>42684</v>
       </c>
       <c r="C87" s="28">
-        <v>0.54015046296296299</v>
+        <v>0.54112268518518525</v>
       </c>
       <c r="D87" s="35">
         <v>42684</v>
       </c>
       <c r="E87" s="28">
-        <v>0.54094907407407411</v>
+        <v>0.54126157407407405</v>
       </c>
       <c r="F87" s="36">
-        <f t="shared" si="1"/>
-        <v>7.9861111111112493E-4</v>
-      </c>
-      <c r="G87" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.3888888888879958E-4</v>
+      </c>
+      <c r="G87" s="41">
+        <f t="shared" si="5"/>
+        <v>11.999999999992284</v>
+      </c>
+      <c r="L87" s="45">
+        <f t="shared" si="6"/>
+        <v>1.0416666666668295E-4</v>
+      </c>
+      <c r="M87" s="43">
+        <f t="shared" si="7"/>
+        <v>9.0000000000014069</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
         <v>85</v>
       </c>
@@ -2968,23 +3806,32 @@
         <v>42684</v>
       </c>
       <c r="C88" s="28">
-        <v>0.54112268518518525</v>
+        <v>0.54136574074074073</v>
       </c>
       <c r="D88" s="35">
         <v>42684</v>
       </c>
       <c r="E88" s="28">
-        <v>0.54126157407407405</v>
+        <v>0.54199074074074072</v>
       </c>
       <c r="F88" s="36">
-        <f t="shared" si="1"/>
-        <v>1.3888888888879958E-4</v>
-      </c>
-      <c r="G88" s="42">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.2499999999998668E-4</v>
+      </c>
+      <c r="G88" s="41">
+        <f t="shared" si="5"/>
+        <v>53.999999999998849</v>
+      </c>
+      <c r="L88" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M88" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
         <v>86</v>
       </c>
@@ -2992,23 +3839,32 @@
         <v>42684</v>
       </c>
       <c r="C89" s="28">
-        <v>0.54136574074074073</v>
+        <v>0.54201388888888891</v>
       </c>
       <c r="D89" s="35">
         <v>42684</v>
       </c>
       <c r="E89" s="28">
-        <v>0.54199074074074072</v>
+        <v>0.54259259259259263</v>
       </c>
       <c r="F89" s="36">
-        <f t="shared" si="1"/>
-        <v>6.2499999999998668E-4</v>
-      </c>
-      <c r="G89" s="42">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>5.7870370370372015E-4</v>
+      </c>
+      <c r="G89" s="41">
+        <f t="shared" si="5"/>
+        <v>50.000000000001421</v>
+      </c>
+      <c r="L89" s="45">
+        <f t="shared" si="6"/>
+        <v>3.240740740739767E-4</v>
+      </c>
+      <c r="M89" s="43">
+        <f t="shared" si="7"/>
+        <v>27.999999999991587</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
         <v>87</v>
       </c>
@@ -3016,23 +3872,32 @@
         <v>42684</v>
       </c>
       <c r="C90" s="28">
-        <v>0.54201388888888891</v>
+        <v>0.5429166666666666</v>
       </c>
       <c r="D90" s="35">
         <v>42684</v>
       </c>
       <c r="E90" s="28">
-        <v>0.54259259259259263</v>
+        <v>0.54309027777777774</v>
       </c>
       <c r="F90" s="36">
-        <f t="shared" si="1"/>
-        <v>5.7870370370372015E-4</v>
-      </c>
-      <c r="G90" s="42">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.7361111111113825E-4</v>
+      </c>
+      <c r="G90" s="41">
+        <f t="shared" si="5"/>
+        <v>15.000000000002345</v>
+      </c>
+      <c r="L90" s="45">
+        <f t="shared" si="6"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="M90" s="43">
+        <f t="shared" si="7"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
         <v>88</v>
       </c>
@@ -3040,23 +3905,32 @@
         <v>42684</v>
       </c>
       <c r="C91" s="28">
-        <v>0.5429166666666666</v>
+        <v>0.54312499999999997</v>
       </c>
       <c r="D91" s="35">
         <v>42684</v>
       </c>
       <c r="E91" s="28">
-        <v>0.54309027777777774</v>
+        <v>0.54402777777777778</v>
       </c>
       <c r="F91" s="36">
-        <f t="shared" si="1"/>
-        <v>1.7361111111113825E-4</v>
-      </c>
-      <c r="G91" s="42">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>9.0277777777780788E-4</v>
+      </c>
+      <c r="G91" s="41">
+        <f t="shared" si="5"/>
+        <v>78.000000000002601</v>
+      </c>
+      <c r="L91" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M91" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
         <v>89</v>
       </c>
@@ -3064,23 +3938,32 @@
         <v>42684</v>
       </c>
       <c r="C92" s="28">
-        <v>0.54312499999999997</v>
+        <v>0.54405092592592597</v>
       </c>
       <c r="D92" s="35">
         <v>42684</v>
       </c>
       <c r="E92" s="28">
-        <v>0.54402777777777778</v>
+        <v>0.54452546296296289</v>
       </c>
       <c r="F92" s="36">
-        <f t="shared" si="1"/>
-        <v>9.0277777777780788E-4</v>
-      </c>
-      <c r="G92" s="42">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.7453703703692618E-4</v>
+      </c>
+      <c r="G92" s="41">
+        <f t="shared" si="5"/>
+        <v>40.999999999990422</v>
+      </c>
+      <c r="L92" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M92" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
         <v>90</v>
       </c>
@@ -3088,23 +3971,32 @@
         <v>42684</v>
       </c>
       <c r="C93" s="28">
-        <v>0.54405092592592597</v>
+        <v>0.54454861111111108</v>
       </c>
       <c r="D93" s="35">
         <v>42684</v>
       </c>
       <c r="E93" s="28">
-        <v>0.54452546296296289</v>
+        <v>0.54533564814814817</v>
       </c>
       <c r="F93" s="36">
-        <f t="shared" si="1"/>
-        <v>4.7453703703692618E-4</v>
-      </c>
-      <c r="G93" s="42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.8703703703708605E-4</v>
+      </c>
+      <c r="G93" s="41">
+        <f t="shared" si="5"/>
+        <v>68.000000000004235</v>
+      </c>
+      <c r="L93" s="45">
+        <f t="shared" si="6"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="M93" s="43">
+        <f t="shared" si="7"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
         <v>91</v>
       </c>
@@ -3112,23 +4004,32 @@
         <v>42684</v>
       </c>
       <c r="C94" s="28">
-        <v>0.54454861111111108</v>
+        <v>0.54535879629629636</v>
       </c>
       <c r="D94" s="35">
         <v>42684</v>
       </c>
       <c r="E94" s="28">
-        <v>0.54533564814814817</v>
+        <v>0.54579861111111116</v>
       </c>
       <c r="F94" s="36">
-        <f t="shared" si="1"/>
-        <v>7.8703703703708605E-4</v>
-      </c>
-      <c r="G94" s="42">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>4.3981481481480955E-4</v>
+      </c>
+      <c r="G94" s="41">
+        <f t="shared" si="5"/>
+        <v>37.999999999999545</v>
+      </c>
+      <c r="L94" s="45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M94" s="43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
         <v>92</v>
       </c>
@@ -3136,23 +4037,32 @@
         <v>42684</v>
       </c>
       <c r="C95" s="28">
-        <v>0.54535879629629636</v>
+        <v>0.54579861111111116</v>
       </c>
       <c r="D95" s="35">
         <v>42684</v>
       </c>
       <c r="E95" s="28">
-        <v>0.54579861111111116</v>
+        <v>0.54615740740740748</v>
       </c>
       <c r="F95" s="36">
-        <f t="shared" si="1"/>
-        <v>4.3981481481480955E-4</v>
-      </c>
-      <c r="G95" s="42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.5879629629631538E-4</v>
+      </c>
+      <c r="G95" s="41">
+        <f t="shared" si="5"/>
+        <v>31.000000000001648</v>
+      </c>
+      <c r="L95" s="45">
+        <f t="shared" si="6"/>
+        <v>3.4722222222116628E-5</v>
+      </c>
+      <c r="M95" s="43">
+        <f t="shared" si="7"/>
+        <v>2.9999999999908766</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
         <v>93</v>
       </c>
@@ -3160,23 +4070,32 @@
         <v>42684</v>
       </c>
       <c r="C96" s="28">
-        <v>0.54579861111111116</v>
+        <v>0.5461921296296296</v>
       </c>
       <c r="D96" s="35">
         <v>42684</v>
       </c>
       <c r="E96" s="28">
-        <v>0.54615740740740748</v>
+        <v>0.54638888888888892</v>
       </c>
       <c r="F96" s="36">
-        <f t="shared" si="1"/>
-        <v>3.5879629629631538E-4</v>
-      </c>
-      <c r="G96" s="42">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.9675925925932702E-4</v>
+      </c>
+      <c r="G96" s="41">
+        <f t="shared" si="5"/>
+        <v>17.000000000005855</v>
+      </c>
+      <c r="L96" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="M96" s="43">
+        <f t="shared" si="7"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
         <v>94</v>
       </c>
@@ -3184,23 +4103,32 @@
         <v>42684</v>
       </c>
       <c r="C97" s="28">
-        <v>0.5461921296296296</v>
+        <v>0.54640046296296296</v>
       </c>
       <c r="D97" s="35">
         <v>42684</v>
       </c>
       <c r="E97" s="28">
-        <v>0.54638888888888892</v>
+        <v>0.54673611111111109</v>
       </c>
       <c r="F97" s="36">
-        <f t="shared" si="1"/>
-        <v>1.9675925925932702E-4</v>
-      </c>
-      <c r="G97" s="42">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.356481481481266E-4</v>
+      </c>
+      <c r="G97" s="41">
+        <f t="shared" si="5"/>
+        <v>28.999999999998138</v>
+      </c>
+      <c r="L97" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M97" s="43">
+        <f t="shared" si="7"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="27">
         <v>95</v>
       </c>
@@ -3208,23 +4136,32 @@
         <v>42684</v>
       </c>
       <c r="C98" s="28">
-        <v>0.54640046296296296</v>
+        <v>0.54674768518518524</v>
       </c>
       <c r="D98" s="35">
         <v>42684</v>
       </c>
       <c r="E98" s="28">
-        <v>0.54673611111111109</v>
+        <v>0.54700231481481476</v>
       </c>
       <c r="F98" s="36">
-        <f t="shared" si="1"/>
-        <v>3.356481481481266E-4</v>
-      </c>
-      <c r="G98" s="42">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.546296296295214E-4</v>
+      </c>
+      <c r="G98" s="41">
+        <f t="shared" si="5"/>
+        <v>21.999999999990649</v>
+      </c>
+      <c r="L98" s="45">
+        <f t="shared" si="6"/>
+        <v>1.1574074074149898E-5</v>
+      </c>
+      <c r="M98" s="43">
+        <f t="shared" si="7"/>
+        <v>1.0000000000065512</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="27">
         <v>96</v>
       </c>
@@ -3232,23 +4169,32 @@
         <v>42684</v>
       </c>
       <c r="C99" s="28">
-        <v>0.54674768518518524</v>
+        <v>0.54701388888888891</v>
       </c>
       <c r="D99" s="35">
         <v>42684</v>
       </c>
       <c r="E99" s="28">
-        <v>0.54700231481481476</v>
+        <v>0.54723379629629632</v>
       </c>
       <c r="F99" s="36">
-        <f t="shared" si="1"/>
-        <v>2.546296296295214E-4</v>
-      </c>
-      <c r="G99" s="42">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.1990740740740478E-4</v>
+      </c>
+      <c r="G99" s="41">
+        <f t="shared" si="5"/>
+        <v>18.999999999999773</v>
+      </c>
+      <c r="L99" s="45">
+        <f t="shared" si="6"/>
+        <v>1.8518518518517713E-4</v>
+      </c>
+      <c r="M99" s="43">
+        <f t="shared" si="7"/>
+        <v>15.999999999999304</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="27">
         <v>97</v>
       </c>
@@ -3256,23 +4202,32 @@
         <v>42684</v>
       </c>
       <c r="C100" s="28">
-        <v>0.54701388888888891</v>
+        <v>0.54741898148148149</v>
       </c>
       <c r="D100" s="35">
         <v>42684</v>
       </c>
       <c r="E100" s="28">
-        <v>0.54723379629629632</v>
+        <v>0.54775462962962962</v>
       </c>
       <c r="F100" s="36">
-        <f t="shared" si="1"/>
-        <v>2.1990740740740478E-4</v>
-      </c>
-      <c r="G100" s="42">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>3.356481481481266E-4</v>
+      </c>
+      <c r="G100" s="41">
+        <f t="shared" si="5"/>
+        <v>28.999999999998138</v>
+      </c>
+      <c r="L100" s="45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M100" s="43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
         <v>98</v>
       </c>
@@ -3280,61 +4235,90 @@
         <v>42684</v>
       </c>
       <c r="C101" s="28">
-        <v>0.54741898148148149</v>
+        <v>0.54775462962962962</v>
       </c>
       <c r="D101" s="35">
         <v>42684</v>
       </c>
       <c r="E101" s="28">
-        <v>0.54775462962962962</v>
+        <v>0.54837962962962961</v>
       </c>
       <c r="F101" s="36">
-        <f t="shared" si="1"/>
-        <v>3.356481481481266E-4</v>
-      </c>
-      <c r="G101" s="42">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.2499999999998668E-4</v>
+      </c>
+      <c r="G101" s="41">
+        <f t="shared" si="5"/>
+        <v>53.999999999998849</v>
+      </c>
+      <c r="L101" s="45">
+        <f t="shared" si="6"/>
+        <v>4.6296296296377548E-5</v>
+      </c>
+      <c r="M101" s="43">
+        <f t="shared" si="7"/>
+        <v>4.0000000000070202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="27">
         <v>99</v>
       </c>
-      <c r="B102" s="35">
-        <v>42684</v>
-      </c>
+      <c r="B102" s="28"/>
       <c r="C102" s="28">
-        <v>0.54775462962962962</v>
-      </c>
-      <c r="D102" s="35">
-        <v>42684</v>
-      </c>
+        <v>0.54842592592592598</v>
+      </c>
+      <c r="D102" s="28"/>
       <c r="E102" s="28">
-        <v>0.54837962962962961</v>
+        <v>0.54925925925925922</v>
       </c>
       <c r="F102" s="36">
-        <f t="shared" si="1"/>
-        <v>6.2499999999998668E-4</v>
-      </c>
-      <c r="G102" s="42">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="27">
+        <f>E102-C102</f>
+        <v>8.3333333333324155E-4</v>
+      </c>
+      <c r="G102" s="41">
+        <f t="shared" si="5"/>
+        <v>71.99999999999207</v>
+      </c>
+      <c r="L102" s="45">
+        <f t="shared" si="6"/>
+        <v>6.94444444444553E-5</v>
+      </c>
+      <c r="M102" s="43">
+        <f t="shared" si="7"/>
+        <v>6.0000000000009379</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="44">
         <v>100</v>
       </c>
-      <c r="B103" s="35"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="28"/>
+      <c r="B103" s="45"/>
+      <c r="C103" s="45">
+        <v>0.54932870370370368</v>
+      </c>
+      <c r="D103" s="45"/>
+      <c r="E103" s="45">
+        <v>0.55027777777777775</v>
+      </c>
       <c r="F103" s="36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G103" s="42">
-        <v>0</v>
-      </c>
+        <f>E103-C103</f>
+        <v>9.490740740740744E-4</v>
+      </c>
+      <c r="G103" s="41">
+        <f t="shared" si="5"/>
+        <v>82.000000000000028</v>
+      </c>
+      <c r="L103" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="M103" s="43">
+        <f>COUNT(M4:M102)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L104" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3351,7 +4335,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4190,7 +5174,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,7 +6014,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,8 +6849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6893,4 +7877,925 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="33">
+        <v>0.63468749999999996</v>
+      </c>
+      <c r="B1" s="33">
+        <f>A2-A1</f>
+        <v>2.1990740740740478E-4</v>
+      </c>
+      <c r="C1" s="43">
+        <f>B1*86400</f>
+        <v>18.999999999999773</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>0.63490740740740736</v>
+      </c>
+      <c r="B2" s="33">
+        <f t="shared" ref="B2:B39" si="0">A3-A2</f>
+        <v>1.1226851851852127E-3</v>
+      </c>
+      <c r="C2" s="43">
+        <f t="shared" ref="C2:C39" si="1">B2*86400</f>
+        <v>97.000000000002373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>0.63603009259259258</v>
+      </c>
+      <c r="B3" s="33">
+        <f t="shared" si="0"/>
+        <v>6.94444444444553E-5</v>
+      </c>
+      <c r="C3" s="43">
+        <f t="shared" si="1"/>
+        <v>6.0000000000009379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>0.63609953703703703</v>
+      </c>
+      <c r="B4" s="33">
+        <f t="shared" si="0"/>
+        <v>2.083333333333659E-4</v>
+      </c>
+      <c r="C4" s="43">
+        <f t="shared" si="1"/>
+        <v>18.000000000002814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>0.6363078703703704</v>
+      </c>
+      <c r="B5" s="33">
+        <f t="shared" si="0"/>
+        <v>3.7037037037035425E-4</v>
+      </c>
+      <c r="C5" s="43">
+        <f t="shared" si="1"/>
+        <v>31.999999999998607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>0.63667824074074075</v>
+      </c>
+      <c r="B6" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1111111111110628E-3</v>
+      </c>
+      <c r="C6" s="43">
+        <f t="shared" si="1"/>
+        <v>95.999999999995822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>0.63778935185185182</v>
+      </c>
+      <c r="B7" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C7" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>0.6378125</v>
+      </c>
+      <c r="B8" s="33">
+        <f t="shared" si="0"/>
+        <v>1.2731481481487172E-4</v>
+      </c>
+      <c r="C8" s="43">
+        <f t="shared" si="1"/>
+        <v>11.000000000004917</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>0.63793981481481488</v>
+      </c>
+      <c r="B9" s="33">
+        <f t="shared" si="0"/>
+        <v>1.5046296296294948E-4</v>
+      </c>
+      <c r="C9" s="43">
+        <f t="shared" si="1"/>
+        <v>12.999999999998835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>0.63809027777777783</v>
+      </c>
+      <c r="B10" s="33">
+        <f t="shared" si="0"/>
+        <v>8.1018518518494176E-5</v>
+      </c>
+      <c r="C10" s="43">
+        <f t="shared" si="1"/>
+        <v>6.9999999999978968</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>0.63817129629629632</v>
+      </c>
+      <c r="B11" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="C11" s="43">
+        <f t="shared" si="1"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>0.63818287037037036</v>
+      </c>
+      <c r="B12" s="33">
+        <f t="shared" si="0"/>
+        <v>1.5046296296294948E-4</v>
+      </c>
+      <c r="C12" s="43">
+        <f t="shared" si="1"/>
+        <v>12.999999999998835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>0.63833333333333331</v>
+      </c>
+      <c r="B13" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C13" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>0.6383564814814815</v>
+      </c>
+      <c r="B14" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C14" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>0.63837962962962969</v>
+      </c>
+      <c r="B15" s="33">
+        <f t="shared" si="0"/>
+        <v>1.96759259259216E-4</v>
+      </c>
+      <c r="C15" s="43">
+        <f t="shared" si="1"/>
+        <v>16.999999999996263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>0.6385763888888889</v>
+      </c>
+      <c r="B16" s="33">
+        <f t="shared" si="0"/>
+        <v>5.7870370370305402E-5</v>
+      </c>
+      <c r="C16" s="43">
+        <f t="shared" si="1"/>
+        <v>4.9999999999943867</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>0.63863425925925921</v>
+      </c>
+      <c r="B17" s="33">
+        <f t="shared" si="0"/>
+        <v>4.3981481481480955E-4</v>
+      </c>
+      <c r="C17" s="43">
+        <f t="shared" si="1"/>
+        <v>37.999999999999545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>0.63907407407407402</v>
+      </c>
+      <c r="B18" s="33">
+        <f t="shared" si="0"/>
+        <v>2.5462962962974345E-4</v>
+      </c>
+      <c r="C18" s="43">
+        <f t="shared" si="1"/>
+        <v>22.000000000009834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>0.63932870370370376</v>
+      </c>
+      <c r="B19" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1574074074038876E-5</v>
+      </c>
+      <c r="C19" s="43">
+        <f t="shared" si="1"/>
+        <v>0.99999999999695888</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>0.6393402777777778</v>
+      </c>
+      <c r="B20" s="33">
+        <f t="shared" si="0"/>
+        <v>2.777777777778212E-4</v>
+      </c>
+      <c r="C20" s="43">
+        <f t="shared" si="1"/>
+        <v>24.000000000003752</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>0.63961805555555562</v>
+      </c>
+      <c r="B21" s="33">
+        <f t="shared" si="0"/>
+        <v>4.9768518518511495E-4</v>
+      </c>
+      <c r="C21" s="43">
+        <f t="shared" si="1"/>
+        <v>42.999999999993932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="33">
+        <v>0.64011574074074074</v>
+      </c>
+      <c r="B22" s="33">
+        <f t="shared" si="0"/>
+        <v>6.3657407407402555E-4</v>
+      </c>
+      <c r="C22" s="43">
+        <f t="shared" si="1"/>
+        <v>54.999999999995808</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <v>0.64075231481481476</v>
+      </c>
+      <c r="B23" s="33">
+        <f t="shared" si="0"/>
+        <v>4.9768518518522598E-4</v>
+      </c>
+      <c r="C23" s="43">
+        <f t="shared" si="1"/>
+        <v>43.000000000003524</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="33">
+        <v>0.64124999999999999</v>
+      </c>
+      <c r="B24" s="33">
+        <f t="shared" si="0"/>
+        <v>2.5462962962963243E-4</v>
+      </c>
+      <c r="C24" s="43">
+        <f t="shared" si="1"/>
+        <v>22.000000000000242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="33">
+        <v>0.64150462962962962</v>
+      </c>
+      <c r="B25" s="33">
+        <f t="shared" si="0"/>
+        <v>2.1990740740740478E-4</v>
+      </c>
+      <c r="C25" s="43">
+        <f t="shared" si="1"/>
+        <v>18.999999999999773</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="33">
+        <v>0.64172453703703702</v>
+      </c>
+      <c r="B26" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C26" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="33">
+        <v>0.64174768518518521</v>
+      </c>
+      <c r="B27" s="33">
+        <f t="shared" si="0"/>
+        <v>1.273148148147607E-4</v>
+      </c>
+      <c r="C27" s="43">
+        <f t="shared" si="1"/>
+        <v>10.999999999995325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="33">
+        <v>0.64187499999999997</v>
+      </c>
+      <c r="B28" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C28" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="33">
+        <v>0.64189814814814816</v>
+      </c>
+      <c r="B29" s="33">
+        <f t="shared" si="0"/>
+        <v>3.472222222222765E-4</v>
+      </c>
+      <c r="C29" s="43">
+        <f t="shared" si="1"/>
+        <v>30.00000000000469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <v>0.64224537037037044</v>
+      </c>
+      <c r="B30" s="33">
+        <f t="shared" si="0"/>
+        <v>2.0833333333325488E-4</v>
+      </c>
+      <c r="C30" s="43">
+        <f t="shared" si="1"/>
+        <v>17.999999999993221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
+        <v>0.64245370370370369</v>
+      </c>
+      <c r="B31" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1342592592592515E-3</v>
+      </c>
+      <c r="C31" s="43">
+        <f t="shared" si="1"/>
+        <v>97.999999999999332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <v>0.64358796296296295</v>
+      </c>
+      <c r="B32" s="33">
+        <f t="shared" si="0"/>
+        <v>4.6296296296299833E-4</v>
+      </c>
+      <c r="C32" s="43">
+        <f t="shared" si="1"/>
+        <v>40.000000000003055</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
+        <v>0.64405092592592594</v>
+      </c>
+      <c r="B33" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C33" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <v>0.64407407407407413</v>
+      </c>
+      <c r="B34" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148077752E-5</v>
+      </c>
+      <c r="C34" s="43">
+        <f t="shared" si="1"/>
+        <v>1.9999999999939178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="33">
+        <v>0.64409722222222221</v>
+      </c>
+      <c r="B35" s="33">
+        <f t="shared" si="0"/>
+        <v>8.1018518518494176E-5</v>
+      </c>
+      <c r="C35" s="43">
+        <f t="shared" si="1"/>
+        <v>6.9999999999978968</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <v>0.6441782407407407</v>
+      </c>
+      <c r="B36" s="33">
+        <f t="shared" si="0"/>
+        <v>3.472222222222765E-5</v>
+      </c>
+      <c r="C36" s="43">
+        <f t="shared" si="1"/>
+        <v>3.000000000000469</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="33">
+        <v>0.64421296296296293</v>
+      </c>
+      <c r="B37" s="33">
+        <f t="shared" si="0"/>
+        <v>6.94444444444553E-5</v>
+      </c>
+      <c r="C37" s="43">
+        <f t="shared" si="1"/>
+        <v>6.0000000000009379</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <v>0.64428240740740739</v>
+      </c>
+      <c r="B38" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3148148148188774E-5</v>
+      </c>
+      <c r="C38" s="43">
+        <f t="shared" si="1"/>
+        <v>2.0000000000035101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>0.64430555555555558</v>
+      </c>
+      <c r="B39" s="33">
+        <f t="shared" si="0"/>
+        <v>-0.64430555555555558</v>
+      </c>
+      <c r="C39" s="43">
+        <f t="shared" si="1"/>
+        <v>-55668</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="33"/>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>COUNTIF(B1:B55,1)</f>
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <f>E4*100/E1</f>
+        <v>67.272727272727266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f>COUNTIF(B1:B55,2)</f>
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <f>E5*100/E1</f>
+        <v>23.636363636363637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <f>COUNTIF(B1:B55,3)</f>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f>E6*100/E1</f>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <f>SUM(F4:F6)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>SUM(E4:E6)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pridane zmeny za pondelok
</commit_message>
<xml_diff>
--- a/data-supermarket.xlsx
+++ b/data-supermarket.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="890" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Obsluha na pokladni" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="VAL - Doba čakania v rade" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="cas_v_systeme_Katka" localSheetId="4">'VAL - Pobyt v systéme'!$B$24:$C$31</definedName>
     <definedName name="dlzkaRadu" localSheetId="5">'VAL - Dĺžka radu pri pokladni'!$B$4:$C$61</definedName>
     <definedName name="doba_obsluhypokladne_1" localSheetId="0">'Obsluha na pokladni'!$B$4:$E$101</definedName>
     <definedName name="New_Text_Document" localSheetId="0">'Obsluha na pokladni'!$G$4:$G$102</definedName>
@@ -38,7 +39,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="dlzkaRadu" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" name="cas_v_systeme_Katka" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\Data\Downloads\cas_v_systeme_Katka.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="dlzkaRadu" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\dlzkaRadu.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -46,7 +55,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="doba_obsluhypokladne" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" name="doba_obsluhypokladne" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\semestralna praca\doba_obsluhypokladne.txt" delimited="0">
       <textFields count="4">
         <textField/>
@@ -56,14 +65,14 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="New Text Document" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" name="New Text Document" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\New Text Document.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="pocet_prichLudi1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" name="pocet_prichLudi1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\pocet_prichLudi.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -71,7 +80,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="pocet_prichLudi2" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" name="pocet_prichLudi2" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="D:\Data\Documents\vysokaSkola\MAS\MAS_billa_simulation\pocet_prichLudi.txt" tab="0" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -83,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Por. Číslo</t>
   </si>
@@ -231,6 +240,15 @@
   <si>
     <t>Confidence Level(95.0%)</t>
   </si>
+  <si>
+    <t>priemer</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
 </sst>
 </file>
 
@@ -288,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,18 +340,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,19 +483,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,16 +506,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
+    <xf numFmtId="21" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,23 +547,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pocet_prichLudi" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlzkaRadu" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cas_v_systeme_Katka" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlzkaRadu" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,7 +836,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,14 +858,14 @@
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="54"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -907,8 +917,18 @@
         <f>F4*86400</f>
         <v>47.000000000005748</v>
       </c>
-      <c r="I4" s="22"/>
+      <c r="I4" s="22">
+        <f>AVERAGE(G4:G103)</f>
+        <v>45.330000000000219</v>
+      </c>
       <c r="J4" s="22"/>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <f>MIN(G4:G103)</f>
+        <v>4.9999999999991829</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -936,6 +956,13 @@
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <f>MAX(G4:G103)</f>
+        <v>146.00000000000205</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -3430,8 +3457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,10 +3478,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3517,7 +3544,7 @@
       </c>
       <c r="D5" s="26"/>
       <c r="E5">
-        <f t="shared" ref="E4:E67" si="1">IF(C5&gt;2,C5,0)</f>
+        <f t="shared" ref="E5:E67" si="1">IF(C5&gt;2,C5,0)</f>
         <v>2.9999999999956728</v>
       </c>
       <c r="H5">
@@ -3544,10 +3571,10 @@
       <c r="H6">
         <v>8</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="58"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -3996,10 +4023,10 @@
       <c r="H23">
         <v>10</v>
       </c>
-      <c r="K23" s="57" t="s">
+      <c r="K23" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="57">
+      <c r="L23" s="49">
         <v>5.9207449317565866</v>
       </c>
     </row>
@@ -5404,7 +5431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -5435,13 +5462,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+      <c r="A3" s="41">
         <v>1</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="40">
         <v>0.63468749999999996</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="42">
         <f>B4-B3</f>
         <v>2.1990740740740478E-4</v>
       </c>
@@ -5451,13 +5478,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="47">
+      <c r="A4" s="41">
         <v>2</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="40">
         <v>0.63490740740740736</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="42">
         <f t="shared" ref="C4:C40" si="0">B5-B4</f>
         <v>1.1226851851852127E-3</v>
       </c>
@@ -5467,13 +5494,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="47">
+      <c r="A5" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="40">
         <v>0.63603009259259258</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="42">
         <f t="shared" si="0"/>
         <v>6.94444444444553E-5</v>
       </c>
@@ -5483,13 +5510,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="47">
+      <c r="A6" s="41">
         <v>4</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="40">
         <v>0.63609953703703703</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="42">
         <f t="shared" si="0"/>
         <v>2.083333333333659E-4</v>
       </c>
@@ -5499,13 +5526,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="A7" s="41">
         <v>5</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="40">
         <v>0.6363078703703704</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="42">
         <f t="shared" si="0"/>
         <v>3.7037037037035425E-4</v>
       </c>
@@ -5515,13 +5542,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
+      <c r="A8" s="41">
         <v>6</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="40">
         <v>0.63667824074074075</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="42">
         <f t="shared" si="0"/>
         <v>1.1111111111110628E-3</v>
       </c>
@@ -5531,13 +5558,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="41">
         <v>7</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="40">
         <v>0.63778935185185182</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5547,13 +5574,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="41">
         <v>8</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="40">
         <v>0.6378125</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="42">
         <f t="shared" si="0"/>
         <v>1.2731481481487172E-4</v>
       </c>
@@ -5563,13 +5590,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="41">
         <v>9</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="40">
         <v>0.63793981481481488</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="42">
         <f t="shared" si="0"/>
         <v>1.5046296296294948E-4</v>
       </c>
@@ -5579,13 +5606,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="41">
         <v>10</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="40">
         <v>0.63809027777777783</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="42">
         <f t="shared" si="0"/>
         <v>8.1018518518494176E-5</v>
       </c>
@@ -5595,13 +5622,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="41">
         <v>11</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="40">
         <v>0.63817129629629632</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="42">
         <f t="shared" si="0"/>
         <v>1.1574074074038876E-5</v>
       </c>
@@ -5611,13 +5638,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="47">
+      <c r="A14" s="41">
         <v>12</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="40">
         <v>0.63818287037037036</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="42">
         <f t="shared" si="0"/>
         <v>1.5046296296294948E-4</v>
       </c>
@@ -5627,13 +5654,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="41">
         <v>13</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B15" s="40">
         <v>0.63833333333333331</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5643,13 +5670,13 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="47">
+      <c r="A16" s="41">
         <v>14</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B16" s="40">
         <v>0.6383564814814815</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5659,13 +5686,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="A17" s="41">
         <v>15</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="40">
         <v>0.63837962962962969</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="42">
         <f t="shared" si="0"/>
         <v>1.96759259259216E-4</v>
       </c>
@@ -5675,13 +5702,13 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47">
+      <c r="A18" s="41">
         <v>16</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="40">
         <v>0.6385763888888889</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="42">
         <f t="shared" si="0"/>
         <v>5.7870370370305402E-5</v>
       </c>
@@ -5691,13 +5718,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="41">
         <v>17</v>
       </c>
-      <c r="B19" s="45">
+      <c r="B19" s="40">
         <v>0.63863425925925921</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="42">
         <f t="shared" si="0"/>
         <v>4.3981481481480955E-4</v>
       </c>
@@ -5707,13 +5734,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47">
+      <c r="A20" s="41">
         <v>18</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="40">
         <v>0.63907407407407402</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="42">
         <f t="shared" si="0"/>
         <v>2.5462962962974345E-4</v>
       </c>
@@ -5723,13 +5750,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47">
+      <c r="A21" s="41">
         <v>19</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B21" s="40">
         <v>0.63932870370370376</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="42">
         <f t="shared" si="0"/>
         <v>1.1574074074038876E-5</v>
       </c>
@@ -5739,13 +5766,13 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47">
+      <c r="A22" s="41">
         <v>20</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B22" s="40">
         <v>0.6393402777777778</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="42">
         <f t="shared" si="0"/>
         <v>2.777777777778212E-4</v>
       </c>
@@ -5755,13 +5782,13 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47">
+      <c r="A23" s="41">
         <v>21</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B23" s="40">
         <v>0.63961805555555562</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="42">
         <f t="shared" si="0"/>
         <v>4.9768518518511495E-4</v>
       </c>
@@ -5771,13 +5798,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="47">
+      <c r="A24" s="41">
         <v>22</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="40">
         <v>0.64011574074074074</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="42">
         <f t="shared" si="0"/>
         <v>6.3657407407402555E-4</v>
       </c>
@@ -5787,13 +5814,13 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="47">
+      <c r="A25" s="41">
         <v>23</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B25" s="40">
         <v>0.64075231481481476</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="42">
         <f t="shared" si="0"/>
         <v>4.9768518518522598E-4</v>
       </c>
@@ -5803,13 +5830,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="47">
+      <c r="A26" s="41">
         <v>24</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="40">
         <v>0.64124999999999999</v>
       </c>
-      <c r="C26" s="48">
+      <c r="C26" s="42">
         <f t="shared" si="0"/>
         <v>2.5462962962963243E-4</v>
       </c>
@@ -5819,13 +5846,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="47">
+      <c r="A27" s="41">
         <v>25</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B27" s="40">
         <v>0.64150462962962962</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="42">
         <f t="shared" si="0"/>
         <v>2.1990740740740478E-4</v>
       </c>
@@ -5835,13 +5862,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="47">
+      <c r="A28" s="41">
         <v>26</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="40">
         <v>0.64172453703703702</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5851,13 +5878,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="47">
+      <c r="A29" s="41">
         <v>27</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B29" s="40">
         <v>0.64174768518518521</v>
       </c>
-      <c r="C29" s="48">
+      <c r="C29" s="42">
         <f t="shared" si="0"/>
         <v>1.273148148147607E-4</v>
       </c>
@@ -5867,13 +5894,13 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="41">
         <v>28</v>
       </c>
-      <c r="B30" s="45">
+      <c r="B30" s="40">
         <v>0.64187499999999997</v>
       </c>
-      <c r="C30" s="48">
+      <c r="C30" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5883,13 +5910,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="47">
+      <c r="A31" s="41">
         <v>29</v>
       </c>
-      <c r="B31" s="45">
+      <c r="B31" s="40">
         <v>0.64189814814814816</v>
       </c>
-      <c r="C31" s="48">
+      <c r="C31" s="42">
         <f t="shared" si="0"/>
         <v>3.472222222222765E-4</v>
       </c>
@@ -5899,13 +5926,13 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47">
+      <c r="A32" s="41">
         <v>30</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="40">
         <v>0.64224537037037044</v>
       </c>
-      <c r="C32" s="48">
+      <c r="C32" s="42">
         <f t="shared" si="0"/>
         <v>2.0833333333325488E-4</v>
       </c>
@@ -5915,13 +5942,13 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="47">
+      <c r="A33" s="41">
         <v>31</v>
       </c>
-      <c r="B33" s="45">
+      <c r="B33" s="40">
         <v>0.64245370370370369</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="42">
         <f t="shared" si="0"/>
         <v>1.1342592592592515E-3</v>
       </c>
@@ -5931,13 +5958,13 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="47">
+      <c r="A34" s="41">
         <v>32</v>
       </c>
-      <c r="B34" s="45">
+      <c r="B34" s="40">
         <v>0.64358796296296295</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="42">
         <f t="shared" si="0"/>
         <v>4.6296296296299833E-4</v>
       </c>
@@ -5947,13 +5974,13 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="47">
+      <c r="A35" s="41">
         <v>33</v>
       </c>
-      <c r="B35" s="45">
+      <c r="B35" s="40">
         <v>0.64405092592592594</v>
       </c>
-      <c r="C35" s="48">
+      <c r="C35" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -5963,13 +5990,13 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="47">
+      <c r="A36" s="41">
         <v>34</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="40">
         <v>0.64407407407407413</v>
       </c>
-      <c r="C36" s="48">
+      <c r="C36" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148077752E-5</v>
       </c>
@@ -5979,13 +6006,13 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="47">
+      <c r="A37" s="41">
         <v>35</v>
       </c>
-      <c r="B37" s="45">
+      <c r="B37" s="40">
         <v>0.64409722222222221</v>
       </c>
-      <c r="C37" s="48">
+      <c r="C37" s="42">
         <f t="shared" si="0"/>
         <v>8.1018518518494176E-5</v>
       </c>
@@ -5995,13 +6022,13 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="47">
+      <c r="A38" s="41">
         <v>36</v>
       </c>
-      <c r="B38" s="45">
+      <c r="B38" s="40">
         <v>0.6441782407407407</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C38" s="42">
         <f t="shared" si="0"/>
         <v>3.472222222222765E-5</v>
       </c>
@@ -6011,13 +6038,13 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="47">
+      <c r="A39" s="41">
         <v>37</v>
       </c>
-      <c r="B39" s="45">
+      <c r="B39" s="40">
         <v>0.64421296296296293</v>
       </c>
-      <c r="C39" s="48">
+      <c r="C39" s="42">
         <f t="shared" si="0"/>
         <v>6.94444444444553E-5</v>
       </c>
@@ -6027,13 +6054,13 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="47">
+      <c r="A40" s="41">
         <v>38</v>
       </c>
-      <c r="B40" s="45">
+      <c r="B40" s="40">
         <v>0.64428240740740739</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C40" s="42">
         <f t="shared" si="0"/>
         <v>2.3148148148188774E-5</v>
       </c>
@@ -6043,13 +6070,13 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="47">
+      <c r="A41" s="41">
         <v>39</v>
       </c>
-      <c r="B41" s="45">
+      <c r="B41" s="40">
         <v>0.64430555555555558</v>
       </c>
-      <c r="C41" s="48"/>
+      <c r="C41" s="42"/>
       <c r="D41" s="17"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -6447,11 +6474,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -6469,7 +6496,7 @@
       <c r="B3" s="33">
         <v>2</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="44" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="31">
@@ -6491,13 +6518,13 @@
       <c r="B5" s="33">
         <v>1</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="45" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6508,14 +6535,14 @@
       <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="46">
         <v>1</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="46">
         <f>COUNTIF(B3:B57,1)</f>
         <v>37</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="46">
         <f>E6*100/E3</f>
         <v>67.272727272727266</v>
       </c>
@@ -6527,14 +6554,14 @@
       <c r="B7" s="33">
         <v>1</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="46">
         <v>2</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="46">
         <f>COUNTIF(B3:B57,2)</f>
         <v>13</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="46">
         <f>E7*100/E3</f>
         <v>23.636363636363637</v>
       </c>
@@ -6546,14 +6573,14 @@
       <c r="B8" s="33">
         <v>1</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="46">
         <v>3</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="46">
         <f>COUNTIF(B3:B57,3)</f>
         <v>5</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="46">
         <f>E8*100/E3</f>
         <v>9.0909090909090917</v>
       </c>
@@ -6565,10 +6592,10 @@
       <c r="B9" s="33">
         <v>2</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="47">
         <f>SUM(F6:F8)</f>
         <v>100</v>
       </c>
@@ -6982,23 +7009,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7008,275 +7035,294 @@
       <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="39">
         <v>0</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="39">
         <v>4.5949074074074078E-3</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="58">
         <f>C3-B3</f>
         <v>4.5949074074074078E-3</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="57">
         <f>D3*86400</f>
         <v>397.00000000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="56">
+        <f>AVERAGE(E3:E31)</f>
+        <v>513.44827586206895</v>
+      </c>
+      <c r="K3">
+        <f>513-156-45</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="39">
         <v>2.8935185185185189E-4</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="39">
         <v>4.2013888888888891E-3</v>
       </c>
-      <c r="D4" s="41">
-        <f t="shared" ref="D4:D23" si="0">C4-B4</f>
+      <c r="D4" s="58">
+        <f t="shared" ref="D4:D31" si="0">C4-B4</f>
         <v>3.9120370370370368E-3</v>
       </c>
-      <c r="E4" s="42">
-        <f t="shared" ref="E4:E23" si="1">D4*86400</f>
+      <c r="E4" s="57">
+        <f t="shared" ref="E4:E31" si="1">D4*86400</f>
         <v>338</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4" s="56">
+        <f>MAX(E3:E31)</f>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="39">
         <v>1.0763888888888889E-3</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="39">
         <v>1.238425925925926E-2</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="58">
         <f t="shared" si="0"/>
         <v>1.1307870370370371E-2</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="57">
         <f t="shared" si="1"/>
         <v>977</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I5" s="56">
+        <f>MIN(E3:E31)</f>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="39">
         <v>1.6203703703703703E-3</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="39">
         <v>7.9861111111111122E-3</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="58">
         <f t="shared" si="0"/>
         <v>6.3657407407407421E-3</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="57">
         <f t="shared" si="1"/>
         <v>550.00000000000011</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="39">
         <v>2.5925925925925925E-3</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="39">
         <v>8.4027777777777781E-3</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="58">
         <f t="shared" si="0"/>
         <v>5.8101851851851856E-3</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="57">
         <f t="shared" si="1"/>
         <v>502.00000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="39">
         <v>6.7129629629629622E-3</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="39">
         <v>9.4212962962962957E-3</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="58">
         <f t="shared" si="0"/>
         <v>2.7083333333333334E-3</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="57">
         <f t="shared" si="1"/>
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="39">
         <v>8.0671296296296307E-3</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="39">
         <v>1.2962962962962963E-2</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="58">
         <f t="shared" si="0"/>
         <v>4.8958333333333319E-3</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="57">
         <f t="shared" si="1"/>
         <v>422.99999999999989</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="39">
         <v>1.0393518518518519E-2</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="39">
         <v>1.8483796296296297E-2</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="58">
         <f t="shared" si="0"/>
         <v>8.0902777777777778E-3</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="57">
         <f t="shared" si="1"/>
         <v>699</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="39">
         <v>1.4120370370370368E-2</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="39">
         <v>2.0034722222222221E-2</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="58">
         <f t="shared" si="0"/>
         <v>5.9143518518518529E-3</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="57">
         <f t="shared" si="1"/>
         <v>511.00000000000011</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="39">
         <v>1.486111111111111E-2</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="39">
         <v>1.9247685185185184E-2</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="58">
         <f t="shared" si="0"/>
         <v>4.386574074074074E-3</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="57">
         <f t="shared" si="1"/>
         <v>379</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="39">
         <v>1.6342592592592593E-2</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="39">
         <v>1.9444444444444445E-2</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="58">
         <f t="shared" si="0"/>
         <v>3.1018518518518522E-3</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="57">
         <f t="shared" si="1"/>
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="39">
         <v>1.8194444444444444E-2</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="39">
         <v>2.298611111111111E-2</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="58">
         <f t="shared" si="0"/>
         <v>4.7916666666666663E-3</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="57">
         <f t="shared" si="1"/>
         <v>413.99999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="39">
         <v>2.0983796296296296E-2</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="39">
         <v>2.6469907407407411E-2</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="58">
         <f t="shared" si="0"/>
         <v>5.4861111111111152E-3</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="57">
         <f t="shared" si="1"/>
         <v>474.00000000000034</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="39">
         <v>0</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="39">
         <v>3.3680555555555551E-3</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="58">
         <f t="shared" si="0"/>
         <v>3.3680555555555551E-3</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="57">
         <f t="shared" si="1"/>
         <v>290.99999999999994</v>
       </c>
@@ -7285,17 +7331,17 @@
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="39">
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="39">
         <v>3.37962962962963E-3</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="58">
         <f t="shared" si="0"/>
         <v>3.368055555555556E-3</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="57">
         <f t="shared" si="1"/>
         <v>291.00000000000006</v>
       </c>
@@ -7304,17 +7350,17 @@
       <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="39">
         <v>1.7361111111111112E-4</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="39">
         <v>7.9976851851851858E-3</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="58">
         <f t="shared" si="0"/>
         <v>7.8240740740740753E-3</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="57">
         <f t="shared" si="1"/>
         <v>676.00000000000011</v>
       </c>
@@ -7323,17 +7369,17 @@
       <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="39">
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="39">
         <v>6.4814814814814813E-3</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="58">
         <f t="shared" si="0"/>
         <v>6.1342592592592594E-3</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="57">
         <f t="shared" si="1"/>
         <v>530</v>
       </c>
@@ -7342,17 +7388,17 @@
       <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="39">
         <v>3.5879629629629635E-4</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="39">
         <v>8.7962962962962968E-3</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="58">
         <f t="shared" si="0"/>
         <v>8.4375000000000006E-3</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="57">
         <f t="shared" si="1"/>
         <v>729</v>
       </c>
@@ -7361,17 +7407,17 @@
       <c r="A21" s="10">
         <v>19</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="39">
         <v>4.3981481481481481E-4</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="39">
         <v>7.0023148148148154E-3</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="58">
         <f t="shared" si="0"/>
         <v>6.5625000000000006E-3</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="57">
         <f t="shared" si="1"/>
         <v>567</v>
       </c>
@@ -7380,17 +7426,17 @@
       <c r="A22" s="10">
         <v>20</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="39">
         <v>8.564814814814815E-4</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="39">
         <v>6.053240740740741E-3</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="58">
         <f t="shared" si="0"/>
         <v>5.1967592592592595E-3</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="57">
         <f t="shared" si="1"/>
         <v>449</v>
       </c>
@@ -7399,17 +7445,17 @@
       <c r="A23" s="10">
         <v>21</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="39">
         <v>1.7245370370370372E-3</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="39">
         <v>5.3240740740740748E-3</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="58">
         <f t="shared" si="0"/>
         <v>3.5995370370370374E-3</v>
       </c>
-      <c r="E23" s="42">
+      <c r="E23" s="57">
         <f t="shared" si="1"/>
         <v>311.00000000000006</v>
       </c>
@@ -7418,73 +7464,153 @@
       <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
+      <c r="B24" s="40">
+        <v>0</v>
+      </c>
+      <c r="C24" s="40">
+        <v>4.9768518518518521E-3</v>
+      </c>
+      <c r="D24" s="58">
+        <f t="shared" si="0"/>
+        <v>4.9768518518518521E-3</v>
+      </c>
+      <c r="E24" s="57">
+        <f t="shared" si="1"/>
+        <v>430</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>23</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
+      <c r="B25" s="40">
+        <v>4.0509259259259258E-4</v>
+      </c>
+      <c r="C25" s="40">
+        <v>8.5416666666666679E-3</v>
+      </c>
+      <c r="D25" s="58">
+        <f t="shared" si="0"/>
+        <v>8.1365740740740756E-3</v>
+      </c>
+      <c r="E25" s="57">
+        <f t="shared" si="1"/>
+        <v>703.00000000000011</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>24</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
+      <c r="B26" s="40">
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="C26" s="40">
+        <v>4.340277777777778E-3</v>
+      </c>
+      <c r="D26" s="58">
+        <f t="shared" si="0"/>
+        <v>3.5069444444444445E-3</v>
+      </c>
+      <c r="E26" s="57">
+        <f t="shared" si="1"/>
+        <v>303</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="B27" s="40">
+        <v>1.0763888888888889E-3</v>
+      </c>
+      <c r="C27" s="40">
+        <v>7.1296296296296307E-3</v>
+      </c>
+      <c r="D27" s="58">
+        <f t="shared" si="0"/>
+        <v>6.0532407407407418E-3</v>
+      </c>
+      <c r="E27" s="57">
+        <f t="shared" si="1"/>
+        <v>523.00000000000011</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>26</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
+      <c r="B28" s="40">
+        <v>1.2152777777777778E-3</v>
+      </c>
+      <c r="C28" s="40">
+        <v>1.6284722222222221E-2</v>
+      </c>
+      <c r="D28" s="58">
+        <f t="shared" si="0"/>
+        <v>1.5069444444444444E-2</v>
+      </c>
+      <c r="E28" s="57">
+        <f t="shared" si="1"/>
+        <v>1302</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>27</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="B29" s="40">
+        <v>1.8402777777777777E-3</v>
+      </c>
+      <c r="C29" s="40">
+        <v>1.1909722222222223E-2</v>
+      </c>
+      <c r="D29" s="58">
+        <f t="shared" si="0"/>
+        <v>1.0069444444444445E-2</v>
+      </c>
+      <c r="E29" s="57">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>28</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+      <c r="B30" s="40">
+        <v>2.4074074074074076E-3</v>
+      </c>
+      <c r="C30" s="40">
+        <v>8.0208333333333329E-3</v>
+      </c>
+      <c r="D30" s="58">
+        <f t="shared" si="0"/>
+        <v>5.6134259259259254E-3</v>
+      </c>
+      <c r="E30" s="57">
+        <f t="shared" si="1"/>
+        <v>484.99999999999994</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>29</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
+      <c r="B31" s="40">
+        <v>2.627314814814815E-3</v>
+      </c>
+      <c r="C31" s="40">
+        <v>5.6828703703703702E-3</v>
+      </c>
+      <c r="D31" s="58">
+        <f t="shared" si="0"/>
+        <v>3.0555555555555553E-3</v>
+      </c>
+      <c r="E31" s="57">
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
@@ -7492,11 +7618,11 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="25"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
@@ -7504,7 +7630,7 @@
       <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="25"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
@@ -7512,7 +7638,7 @@
       <c r="F34" s="26"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="25"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -7520,7 +7646,7 @@
       <c r="F35" s="26"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="25"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
@@ -7528,7 +7654,7 @@
       <c r="F36" s="26"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="25"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
@@ -7536,7 +7662,7 @@
       <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="25"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
@@ -7544,7 +7670,7 @@
       <c r="F38" s="26"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="40"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="25"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -7552,7 +7678,7 @@
       <c r="F39" s="26"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
+      <c r="A40" s="38"/>
       <c r="B40" s="25"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
@@ -7560,7 +7686,7 @@
       <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="25"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
@@ -7568,7 +7694,7 @@
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="25"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -7576,7 +7702,7 @@
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="40"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="25"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -7584,7 +7710,7 @@
       <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="25"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -7592,7 +7718,7 @@
       <c r="F44" s="26"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
+      <c r="A45" s="38"/>
       <c r="B45" s="25"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
@@ -7600,7 +7726,7 @@
       <c r="F45" s="26"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="25"/>
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
@@ -7608,7 +7734,7 @@
       <c r="F46" s="26"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="25"/>
       <c r="C47" s="26"/>
       <c r="D47" s="26"/>
@@ -7616,7 +7742,7 @@
       <c r="F47" s="26"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="25"/>
       <c r="C48" s="26"/>
       <c r="D48" s="26"/>
@@ -7624,7 +7750,7 @@
       <c r="F48" s="26"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="25"/>
       <c r="C49" s="26"/>
       <c r="D49" s="26"/>
@@ -7632,7 +7758,7 @@
       <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="25"/>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
@@ -7640,7 +7766,7 @@
       <c r="F50" s="26"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="25"/>
       <c r="C51" s="26"/>
       <c r="D51" s="26"/>
@@ -7648,7 +7774,7 @@
       <c r="F51" s="26"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="25"/>
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
@@ -7656,7 +7782,7 @@
       <c r="F52" s="26"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="25"/>
       <c r="C53" s="26"/>
       <c r="D53" s="26"/>
@@ -7664,7 +7790,7 @@
       <c r="F53" s="26"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="25"/>
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
@@ -7672,7 +7798,7 @@
       <c r="F54" s="26"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="25"/>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -7680,7 +7806,7 @@
       <c r="F55" s="26"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
+      <c r="A56" s="38"/>
       <c r="B56" s="25"/>
       <c r="C56" s="26"/>
       <c r="D56" s="26"/>
@@ -7688,7 +7814,7 @@
       <c r="F56" s="26"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
+      <c r="A57" s="38"/>
       <c r="B57" s="25"/>
       <c r="C57" s="26"/>
       <c r="D57" s="26"/>
@@ -7696,7 +7822,7 @@
       <c r="F57" s="26"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
+      <c r="A58" s="38"/>
       <c r="B58" s="25"/>
       <c r="C58" s="26"/>
       <c r="D58" s="26"/>
@@ -7704,7 +7830,7 @@
       <c r="F58" s="26"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="25"/>
       <c r="C59" s="26"/>
       <c r="D59" s="26"/>
@@ -7712,7 +7838,7 @@
       <c r="F59" s="26"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
+      <c r="A60" s="38"/>
       <c r="B60" s="25"/>
       <c r="C60" s="26"/>
       <c r="D60" s="26"/>
@@ -7720,7 +7846,7 @@
       <c r="F60" s="26"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="40"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="25"/>
       <c r="C61" s="26"/>
       <c r="D61" s="26"/>
@@ -7728,7 +7854,7 @@
       <c r="F61" s="26"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
+      <c r="A62" s="38"/>
       <c r="B62" s="25"/>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
@@ -7736,7 +7862,7 @@
       <c r="F62" s="26"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
+      <c r="A63" s="38"/>
       <c r="B63" s="25"/>
       <c r="C63" s="26"/>
       <c r="D63" s="26"/>
@@ -7744,7 +7870,7 @@
       <c r="F63" s="26"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
+      <c r="A64" s="38"/>
       <c r="B64" s="25"/>
       <c r="C64" s="26"/>
       <c r="D64" s="26"/>
@@ -7752,7 +7878,7 @@
       <c r="F64" s="26"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="25"/>
       <c r="C65" s="26"/>
       <c r="D65" s="26"/>
@@ -7760,7 +7886,7 @@
       <c r="F65" s="26"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
+      <c r="A66" s="38"/>
       <c r="B66" s="25"/>
       <c r="C66" s="26"/>
       <c r="D66" s="26"/>
@@ -7768,7 +7894,7 @@
       <c r="F66" s="26"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="40"/>
+      <c r="A67" s="38"/>
       <c r="B67" s="25"/>
       <c r="C67" s="26"/>
       <c r="D67" s="26"/>
@@ -7776,7 +7902,7 @@
       <c r="F67" s="26"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
+      <c r="A68" s="38"/>
       <c r="B68" s="25"/>
       <c r="C68" s="26"/>
       <c r="D68" s="26"/>
@@ -7784,7 +7910,7 @@
       <c r="F68" s="26"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="40"/>
+      <c r="A69" s="38"/>
       <c r="B69" s="25"/>
       <c r="C69" s="26"/>
       <c r="D69" s="26"/>
@@ -7792,7 +7918,7 @@
       <c r="F69" s="26"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
+      <c r="A70" s="38"/>
       <c r="B70" s="25"/>
       <c r="C70" s="26"/>
       <c r="D70" s="26"/>
@@ -7800,7 +7926,7 @@
       <c r="F70" s="26"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="40"/>
+      <c r="A71" s="38"/>
       <c r="B71" s="25"/>
       <c r="C71" s="26"/>
       <c r="D71" s="26"/>
@@ -7808,7 +7934,7 @@
       <c r="F71" s="26"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="40"/>
+      <c r="A72" s="38"/>
       <c r="B72" s="25"/>
       <c r="C72" s="26"/>
       <c r="D72" s="26"/>
@@ -7816,7 +7942,7 @@
       <c r="F72" s="26"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="40"/>
+      <c r="A73" s="38"/>
       <c r="B73" s="25"/>
       <c r="C73" s="26"/>
       <c r="D73" s="26"/>
@@ -7824,7 +7950,7 @@
       <c r="F73" s="26"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="40"/>
+      <c r="A74" s="38"/>
       <c r="B74" s="25"/>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -7832,7 +7958,7 @@
       <c r="F74" s="26"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="40"/>
+      <c r="A75" s="38"/>
       <c r="B75" s="25"/>
       <c r="C75" s="26"/>
       <c r="D75" s="26"/>
@@ -7840,7 +7966,7 @@
       <c r="F75" s="26"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="40"/>
+      <c r="A76" s="38"/>
       <c r="B76" s="25"/>
       <c r="C76" s="26"/>
       <c r="D76" s="26"/>
@@ -7848,7 +7974,7 @@
       <c r="F76" s="26"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
+      <c r="A77" s="38"/>
       <c r="B77" s="25"/>
       <c r="C77" s="26"/>
       <c r="D77" s="26"/>
@@ -7856,7 +7982,7 @@
       <c r="F77" s="26"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="40"/>
+      <c r="A78" s="38"/>
       <c r="B78" s="25"/>
       <c r="C78" s="26"/>
       <c r="D78" s="26"/>
@@ -7864,7 +7990,7 @@
       <c r="F78" s="26"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="40"/>
+      <c r="A79" s="38"/>
       <c r="B79" s="25"/>
       <c r="C79" s="26"/>
       <c r="D79" s="26"/>
@@ -7872,7 +7998,7 @@
       <c r="F79" s="26"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="40"/>
+      <c r="A80" s="38"/>
       <c r="B80" s="25"/>
       <c r="C80" s="26"/>
       <c r="D80" s="26"/>
@@ -7880,7 +8006,7 @@
       <c r="F80" s="26"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="40"/>
+      <c r="A81" s="38"/>
       <c r="B81" s="25"/>
       <c r="C81" s="26"/>
       <c r="D81" s="26"/>
@@ -7888,7 +8014,7 @@
       <c r="F81" s="26"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="40"/>
+      <c r="A82" s="38"/>
       <c r="B82" s="25"/>
       <c r="C82" s="26"/>
       <c r="D82" s="26"/>
@@ -7896,7 +8022,7 @@
       <c r="F82" s="26"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="40"/>
+      <c r="A83" s="38"/>
       <c r="B83" s="25"/>
       <c r="C83" s="26"/>
       <c r="D83" s="26"/>
@@ -7904,7 +8030,7 @@
       <c r="F83" s="26"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="40"/>
+      <c r="A84" s="38"/>
       <c r="B84" s="25"/>
       <c r="C84" s="26"/>
       <c r="D84" s="26"/>
@@ -7912,7 +8038,7 @@
       <c r="F84" s="26"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="40"/>
+      <c r="A85" s="38"/>
       <c r="B85" s="25"/>
       <c r="C85" s="26"/>
       <c r="D85" s="26"/>
@@ -7920,7 +8046,7 @@
       <c r="F85" s="26"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="40"/>
+      <c r="A86" s="38"/>
       <c r="B86" s="25"/>
       <c r="C86" s="26"/>
       <c r="D86" s="26"/>
@@ -7928,7 +8054,7 @@
       <c r="F86" s="26"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="40"/>
+      <c r="A87" s="38"/>
       <c r="B87" s="25"/>
       <c r="C87" s="26"/>
       <c r="D87" s="26"/>
@@ -7936,7 +8062,7 @@
       <c r="F87" s="26"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="40"/>
+      <c r="A88" s="38"/>
       <c r="B88" s="25"/>
       <c r="C88" s="26"/>
       <c r="D88" s="26"/>
@@ -7944,7 +8070,7 @@
       <c r="F88" s="26"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="40"/>
+      <c r="A89" s="38"/>
       <c r="B89" s="25"/>
       <c r="C89" s="26"/>
       <c r="D89" s="26"/>
@@ -7952,7 +8078,7 @@
       <c r="F89" s="26"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="40"/>
+      <c r="A90" s="38"/>
       <c r="B90" s="25"/>
       <c r="C90" s="26"/>
       <c r="D90" s="26"/>
@@ -7960,7 +8086,7 @@
       <c r="F90" s="26"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="40"/>
+      <c r="A91" s="38"/>
       <c r="B91" s="25"/>
       <c r="C91" s="26"/>
       <c r="D91" s="26"/>
@@ -7968,7 +8094,7 @@
       <c r="F91" s="26"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="40"/>
+      <c r="A92" s="38"/>
       <c r="B92" s="25"/>
       <c r="C92" s="26"/>
       <c r="D92" s="26"/>
@@ -7976,7 +8102,7 @@
       <c r="F92" s="26"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="40"/>
+      <c r="A93" s="38"/>
       <c r="B93" s="25"/>
       <c r="C93" s="26"/>
       <c r="D93" s="26"/>
@@ -7984,7 +8110,7 @@
       <c r="F93" s="26"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="40"/>
+      <c r="A94" s="38"/>
       <c r="B94" s="25"/>
       <c r="C94" s="26"/>
       <c r="D94" s="26"/>
@@ -7992,7 +8118,7 @@
       <c r="F94" s="26"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="40"/>
+      <c r="A95" s="38"/>
       <c r="B95" s="25"/>
       <c r="C95" s="26"/>
       <c r="D95" s="26"/>
@@ -8000,7 +8126,7 @@
       <c r="F95" s="26"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="40"/>
+      <c r="A96" s="38"/>
       <c r="B96" s="25"/>
       <c r="C96" s="26"/>
       <c r="D96" s="26"/>
@@ -8008,7 +8134,7 @@
       <c r="F96" s="26"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="40"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="25"/>
       <c r="C97" s="26"/>
       <c r="D97" s="26"/>
@@ -8016,7 +8142,7 @@
       <c r="F97" s="26"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="40"/>
+      <c r="A98" s="38"/>
       <c r="B98" s="25"/>
       <c r="C98" s="26"/>
       <c r="D98" s="26"/>
@@ -8024,7 +8150,7 @@
       <c r="F98" s="26"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="40"/>
+      <c r="A99" s="38"/>
       <c r="B99" s="25"/>
       <c r="C99" s="26"/>
       <c r="D99" s="26"/>
@@ -8032,7 +8158,7 @@
       <c r="F99" s="26"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="40"/>
+      <c r="A100" s="38"/>
       <c r="B100" s="25"/>
       <c r="C100" s="26"/>
       <c r="D100" s="26"/>
@@ -8040,7 +8166,7 @@
       <c r="F100" s="26"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="40"/>
+      <c r="A101" s="38"/>
       <c r="B101" s="25"/>
       <c r="C101" s="26"/>
       <c r="D101" s="26"/>
@@ -8048,7 +8174,7 @@
       <c r="F101" s="26"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="40"/>
+      <c r="A102" s="38"/>
       <c r="B102" s="25"/>
       <c r="C102" s="26"/>
       <c r="D102" s="26"/>
@@ -8072,8 +8198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8118,10 +8244,10 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="55">
         <f>COUNT(C4:C61)</f>
         <v>58</v>
       </c>
@@ -8138,10 +8264,10 @@
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="55">
         <f>AVERAGE(C4:C61)</f>
         <v>4.1724137931034484</v>
       </c>
@@ -9268,28 +9394,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-    </row>
-    <row r="2" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+    </row>
+    <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -9299,258 +9426,270 @@
       <c r="C2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="40">
         <v>0</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="40">
         <v>1.8865740740740742E-3</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="42">
         <f>C3-B3</f>
         <v>1.8865740740740742E-3</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="57">
         <f>D3*86400</f>
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="56">
+        <f>AVERAGE(E3:E14)</f>
+        <v>155.91666666666666</v>
+      </c>
+      <c r="I3" s="56">
+        <f>MIN(E3:E14)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="40">
         <v>0</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="40">
         <v>1.6203703703703703E-3</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="42">
         <f t="shared" ref="D4:D14" si="0">C4-B4</f>
         <v>1.6203703703703703E-3</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="57">
         <f t="shared" ref="E4:E14" si="1">D4*86400</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4" s="56">
+        <f>MAX(E3:E14)</f>
+        <v>315.99999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="40">
         <v>3.9351851851851852E-4</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="40">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="42">
         <f t="shared" si="0"/>
         <v>9.9537037037037042E-4</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="57">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="40">
         <v>3.9351851851851852E-4</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="40">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="42">
         <f t="shared" si="0"/>
         <v>2.3842592592592596E-3</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="57">
         <f t="shared" si="1"/>
         <v>206.00000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="40">
         <v>1.1226851851851851E-3</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="40">
         <v>4.7800925925925919E-3</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="42">
         <f t="shared" si="0"/>
         <v>3.657407407407407E-3</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="57">
         <f t="shared" si="1"/>
         <v>315.99999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="40">
         <v>2.5462962962962961E-3</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="40">
         <v>4.363425925925926E-3</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="42">
         <f t="shared" si="0"/>
         <v>1.8171296296296299E-3</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="57">
         <f t="shared" si="1"/>
         <v>157.00000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="40">
         <v>2.9861111111111113E-3</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="40">
         <v>4.5138888888888893E-3</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="42">
         <f t="shared" si="0"/>
         <v>1.5277777777777781E-3</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="57">
         <f t="shared" si="1"/>
         <v>132.00000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="40">
         <v>3.4490740740740745E-3</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="40">
         <v>4.9768518518518521E-3</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="42">
         <f t="shared" si="0"/>
         <v>1.5277777777777776E-3</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="57">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="40">
         <v>5.1273148148148146E-3</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="40">
         <v>7.8125E-3</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="42">
         <f t="shared" si="0"/>
         <v>2.6851851851851854E-3</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="57">
         <f t="shared" si="1"/>
         <v>232.00000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="40">
         <v>5.5671296296296302E-3</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="40">
         <v>6.7129629629629622E-3</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="42">
         <f t="shared" si="0"/>
         <v>1.145833333333332E-3</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="57">
         <f t="shared" si="1"/>
         <v>98.999999999999886</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="40">
         <v>5.7291666666666671E-3</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="40">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="42">
         <f t="shared" si="0"/>
         <v>1.2152777777777769E-3</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="57">
         <f t="shared" si="1"/>
         <v>104.99999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="40">
         <v>7.6388888888888886E-3</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="40">
         <v>8.8310185185185176E-3</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="42">
         <f t="shared" si="0"/>
         <v>1.1921296296296289E-3</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="57">
         <f t="shared" si="1"/>
         <v>102.99999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -9558,8 +9697,8 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -9567,8 +9706,8 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
@@ -9576,8 +9715,8 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -9585,8 +9724,8 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -9594,8 +9733,8 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
@@ -9603,8 +9742,8 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Posledne upravy pred odovzdavim, snad bude plny
</commit_message>
<xml_diff>
--- a/data-supermarket.xlsx
+++ b/data-supermarket.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="890" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="890" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Obsluha na pokladni" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
   <si>
     <t>Por. Číslo</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Dĺžka radu</t>
-  </si>
-  <si>
-    <t>Priemerná dĺžka radu:</t>
   </si>
   <si>
     <t xml:space="preserve">Doba čakania v rade </t>
@@ -329,6 +326,27 @@
   <si>
     <t xml:space="preserve">4 v rade </t>
   </si>
+  <si>
+    <t>Jeden  brigádnik</t>
+  </si>
+  <si>
+    <t>Dvaja brigádnici</t>
+  </si>
+  <si>
+    <t>Traja brigádnici</t>
+  </si>
+  <si>
+    <t>Štyria brigádnici</t>
+  </si>
+  <si>
+    <t>Porovnanie</t>
+  </si>
+  <si>
+    <t>Dvaja v rade pred zákazníkom</t>
+  </si>
+  <si>
+    <t>Štyria v rade pred zákazníkom</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +357,7 @@
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
     <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="170" formatCode="0.0000;[Red]0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000;[Red]0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -490,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -600,20 +618,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,11 +635,27 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,11 +679,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="New Text Document" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="doba_obsluhypokladne_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -967,14 +991,14 @@
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="56"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
@@ -1027,9 +1051,9 @@
         <v>47.000000000005748</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="60">
+        <v>49</v>
+      </c>
+      <c r="J4" s="56">
         <f>MIN(G4:G103)</f>
         <v>4.9999999999991829</v>
       </c>
@@ -1059,9 +1083,9 @@
         <v>99.00000000000108</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="60">
+        <v>50</v>
+      </c>
+      <c r="J5" s="56">
         <f>MAX(G4:G103)</f>
         <v>146.00000000000205</v>
       </c>
@@ -1091,9 +1115,9 @@
         <v>16.0000000000041</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="60">
+        <v>48</v>
+      </c>
+      <c r="J6" s="56">
         <f>AVERAGE(G4:G103)</f>
         <v>45.330000000000219</v>
       </c>
@@ -3679,7 +3703,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" s="49"/>
     </row>
@@ -3727,7 +3751,7 @@
         <v>7</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" s="16">
         <v>10.583333333333334</v>
@@ -3754,7 +3778,7 @@
         <v>12</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L9" s="16">
         <v>2.8621193289484101</v>
@@ -3781,7 +3805,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="16">
         <v>5</v>
@@ -3808,7 +3832,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="16">
         <v>3</v>
@@ -3835,7 +3859,7 @@
         <v>30</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="16">
         <v>14.021463877761207</v>
@@ -3862,7 +3886,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L13" s="16">
         <v>196.60144927536234</v>
@@ -3889,7 +3913,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="16">
         <v>7.8603765496970084</v>
@@ -3916,7 +3940,7 @@
         <v>62</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L15" s="16">
         <v>2.7359311609892436</v>
@@ -3943,7 +3967,7 @@
         <v>38</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" s="16">
         <v>59</v>
@@ -3970,7 +3994,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" s="16">
         <v>3</v>
@@ -3997,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L18" s="16">
         <v>62</v>
@@ -4024,7 +4048,7 @@
         <v>4</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L19" s="16">
         <v>254</v>
@@ -4051,7 +4075,7 @@
         <v>3</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L20" s="16">
         <v>24</v>
@@ -4077,7 +4101,7 @@
         <v>5</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L21" s="16">
         <v>62</v>
@@ -4104,7 +4128,7 @@
         <v>7</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L22" s="16">
         <v>3</v>
@@ -4131,7 +4155,7 @@
         <v>10</v>
       </c>
       <c r="K23" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L23" s="48">
         <v>5.9207449317565866</v>
@@ -6579,11 +6603,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="A1" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -6698,7 +6722,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="46">
         <f>SUM(F6:F8)</f>
@@ -7157,18 +7181,18 @@
       <c r="C3" s="38">
         <v>4.5949074074074078E-3</v>
       </c>
-      <c r="D3" s="55">
+      <c r="D3" s="54">
         <f>C3-B3</f>
         <v>4.5949074074074078E-3</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="53">
         <f>D3*86400</f>
         <v>397.00000000000006</v>
       </c>
-      <c r="G3" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="61">
+      <c r="G3" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="57">
         <f>MAX(E3:E31)</f>
         <v>1302</v>
       </c>
@@ -7183,18 +7207,18 @@
       <c r="C4" s="38">
         <v>4.2013888888888891E-3</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="54">
         <f t="shared" ref="D4:D31" si="0">C4-B4</f>
         <v>3.9120370370370368E-3</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="53">
         <f t="shared" ref="E4:E31" si="1">D4*86400</f>
         <v>338</v>
       </c>
-      <c r="G4" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="61">
+      <c r="G4" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="57">
         <f>MIN(E3:E31)</f>
         <v>234</v>
       </c>
@@ -7209,18 +7233,18 @@
       <c r="C5" s="38">
         <v>1.238425925925926E-2</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="54">
         <f t="shared" si="0"/>
         <v>1.1307870370370371E-2</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="53">
         <f t="shared" si="1"/>
         <v>977</v>
       </c>
-      <c r="G5" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="61">
+      <c r="G5" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="57">
         <f>AVERAGE(E3:E31)</f>
         <v>513.44827586206895</v>
       </c>
@@ -7235,11 +7259,11 @@
       <c r="C6" s="38">
         <v>7.9861111111111122E-3</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="54">
         <f t="shared" si="0"/>
         <v>6.3657407407407421E-3</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="53">
         <f t="shared" si="1"/>
         <v>550.00000000000011</v>
       </c>
@@ -7254,11 +7278,11 @@
       <c r="C7" s="38">
         <v>8.4027777777777781E-3</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="54">
         <f t="shared" si="0"/>
         <v>5.8101851851851856E-3</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="53">
         <f t="shared" si="1"/>
         <v>502.00000000000006</v>
       </c>
@@ -7273,11 +7297,11 @@
       <c r="C8" s="38">
         <v>9.4212962962962957E-3</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="54">
         <f t="shared" si="0"/>
         <v>2.7083333333333334E-3</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="53">
         <f t="shared" si="1"/>
         <v>234</v>
       </c>
@@ -7292,11 +7316,11 @@
       <c r="C9" s="38">
         <v>1.2962962962962963E-2</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="54">
         <f t="shared" si="0"/>
         <v>4.8958333333333319E-3</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="53">
         <f t="shared" si="1"/>
         <v>422.99999999999989</v>
       </c>
@@ -7311,11 +7335,11 @@
       <c r="C10" s="38">
         <v>1.8483796296296297E-2</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="54">
         <f t="shared" si="0"/>
         <v>8.0902777777777778E-3</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="53">
         <f t="shared" si="1"/>
         <v>699</v>
       </c>
@@ -7330,11 +7354,11 @@
       <c r="C11" s="38">
         <v>2.0034722222222221E-2</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="54">
         <f t="shared" si="0"/>
         <v>5.9143518518518529E-3</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="53">
         <f t="shared" si="1"/>
         <v>511.00000000000011</v>
       </c>
@@ -7349,11 +7373,11 @@
       <c r="C12" s="38">
         <v>1.9247685185185184E-2</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="54">
         <f t="shared" si="0"/>
         <v>4.386574074074074E-3</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="53">
         <f t="shared" si="1"/>
         <v>379</v>
       </c>
@@ -7368,11 +7392,11 @@
       <c r="C13" s="38">
         <v>1.9444444444444445E-2</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="54">
         <f t="shared" si="0"/>
         <v>3.1018518518518522E-3</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="53">
         <f t="shared" si="1"/>
         <v>268</v>
       </c>
@@ -7387,11 +7411,11 @@
       <c r="C14" s="38">
         <v>2.298611111111111E-2</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="54">
         <f t="shared" si="0"/>
         <v>4.7916666666666663E-3</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="53">
         <f t="shared" si="1"/>
         <v>413.99999999999994</v>
       </c>
@@ -7406,11 +7430,11 @@
       <c r="C15" s="38">
         <v>2.6469907407407411E-2</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="54">
         <f t="shared" si="0"/>
         <v>5.4861111111111152E-3</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="53">
         <f t="shared" si="1"/>
         <v>474.00000000000034</v>
       </c>
@@ -7425,11 +7449,11 @@
       <c r="C16" s="38">
         <v>3.3680555555555551E-3</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="54">
         <f t="shared" si="0"/>
         <v>3.3680555555555551E-3</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="53">
         <f t="shared" si="1"/>
         <v>290.99999999999994</v>
       </c>
@@ -7444,11 +7468,11 @@
       <c r="C17" s="38">
         <v>3.37962962962963E-3</v>
       </c>
-      <c r="D17" s="55">
+      <c r="D17" s="54">
         <f t="shared" si="0"/>
         <v>3.368055555555556E-3</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="53">
         <f t="shared" si="1"/>
         <v>291.00000000000006</v>
       </c>
@@ -7463,11 +7487,11 @@
       <c r="C18" s="38">
         <v>7.9976851851851858E-3</v>
       </c>
-      <c r="D18" s="55">
+      <c r="D18" s="54">
         <f t="shared" si="0"/>
         <v>7.8240740740740753E-3</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="53">
         <f t="shared" si="1"/>
         <v>676.00000000000011</v>
       </c>
@@ -7482,11 +7506,11 @@
       <c r="C19" s="38">
         <v>6.4814814814814813E-3</v>
       </c>
-      <c r="D19" s="55">
+      <c r="D19" s="54">
         <f t="shared" si="0"/>
         <v>6.1342592592592594E-3</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="53">
         <f t="shared" si="1"/>
         <v>530</v>
       </c>
@@ -7501,11 +7525,11 @@
       <c r="C20" s="38">
         <v>8.7962962962962968E-3</v>
       </c>
-      <c r="D20" s="55">
+      <c r="D20" s="54">
         <f t="shared" si="0"/>
         <v>8.4375000000000006E-3</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="53">
         <f t="shared" si="1"/>
         <v>729</v>
       </c>
@@ -7520,11 +7544,11 @@
       <c r="C21" s="38">
         <v>7.0023148148148154E-3</v>
       </c>
-      <c r="D21" s="55">
+      <c r="D21" s="54">
         <f t="shared" si="0"/>
         <v>6.5625000000000006E-3</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="53">
         <f t="shared" si="1"/>
         <v>567</v>
       </c>
@@ -7539,11 +7563,11 @@
       <c r="C22" s="38">
         <v>6.053240740740741E-3</v>
       </c>
-      <c r="D22" s="55">
+      <c r="D22" s="54">
         <f t="shared" si="0"/>
         <v>5.1967592592592595E-3</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="53">
         <f t="shared" si="1"/>
         <v>449</v>
       </c>
@@ -7558,11 +7582,11 @@
       <c r="C23" s="38">
         <v>5.3240740740740748E-3</v>
       </c>
-      <c r="D23" s="55">
+      <c r="D23" s="54">
         <f t="shared" si="0"/>
         <v>3.5995370370370374E-3</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="53">
         <f t="shared" si="1"/>
         <v>311.00000000000006</v>
       </c>
@@ -7577,11 +7601,11 @@
       <c r="C24" s="39">
         <v>4.9768518518518521E-3</v>
       </c>
-      <c r="D24" s="55">
+      <c r="D24" s="54">
         <f t="shared" si="0"/>
         <v>4.9768518518518521E-3</v>
       </c>
-      <c r="E24" s="54">
+      <c r="E24" s="53">
         <f t="shared" si="1"/>
         <v>430</v>
       </c>
@@ -7596,11 +7620,11 @@
       <c r="C25" s="39">
         <v>8.5416666666666679E-3</v>
       </c>
-      <c r="D25" s="55">
+      <c r="D25" s="54">
         <f t="shared" si="0"/>
         <v>8.1365740740740756E-3</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="53">
         <f t="shared" si="1"/>
         <v>703.00000000000011</v>
       </c>
@@ -7615,11 +7639,11 @@
       <c r="C26" s="39">
         <v>4.340277777777778E-3</v>
       </c>
-      <c r="D26" s="55">
+      <c r="D26" s="54">
         <f t="shared" si="0"/>
         <v>3.5069444444444445E-3</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="53">
         <f t="shared" si="1"/>
         <v>303</v>
       </c>
@@ -7634,11 +7658,11 @@
       <c r="C27" s="39">
         <v>7.1296296296296307E-3</v>
       </c>
-      <c r="D27" s="55">
+      <c r="D27" s="54">
         <f t="shared" si="0"/>
         <v>6.0532407407407418E-3</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="53">
         <f t="shared" si="1"/>
         <v>523.00000000000011</v>
       </c>
@@ -7653,11 +7677,11 @@
       <c r="C28" s="39">
         <v>1.6284722222222221E-2</v>
       </c>
-      <c r="D28" s="55">
+      <c r="D28" s="54">
         <f t="shared" si="0"/>
         <v>1.5069444444444444E-2</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="53">
         <f t="shared" si="1"/>
         <v>1302</v>
       </c>
@@ -7672,11 +7696,11 @@
       <c r="C29" s="39">
         <v>1.1909722222222223E-2</v>
       </c>
-      <c r="D29" s="55">
+      <c r="D29" s="54">
         <f t="shared" si="0"/>
         <v>1.0069444444444445E-2</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="53">
         <f t="shared" si="1"/>
         <v>870</v>
       </c>
@@ -7691,11 +7715,11 @@
       <c r="C30" s="39">
         <v>8.0208333333333329E-3</v>
       </c>
-      <c r="D30" s="55">
+      <c r="D30" s="54">
         <f t="shared" si="0"/>
         <v>5.6134259259259254E-3</v>
       </c>
-      <c r="E30" s="54">
+      <c r="E30" s="53">
         <f t="shared" si="1"/>
         <v>484.99999999999994</v>
       </c>
@@ -7710,11 +7734,11 @@
       <c r="C31" s="39">
         <v>5.6828703703703702E-3</v>
       </c>
-      <c r="D31" s="55">
+      <c r="D31" s="54">
         <f t="shared" si="0"/>
         <v>3.0555555555555553E-3</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="53">
         <f t="shared" si="1"/>
         <v>264</v>
       </c>
@@ -7725,8 +7749,8 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
@@ -8306,7 +8330,7 @@
   <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8337,7 +8361,8 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="11"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
@@ -8347,17 +8372,12 @@
         <v>0.66517361111111117</v>
       </c>
       <c r="C4" s="36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="52">
-        <f>COUNT(C4:C61)</f>
-        <v>58</v>
-      </c>
+      <c r="F4" s="74"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -8371,13 +8391,8 @@
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="52">
-        <f>AVERAGE(C4:C61)</f>
-        <v>4.1724137931034484</v>
-      </c>
+      <c r="F5" s="74"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
@@ -9509,35 +9524,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="A1" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="50" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -9554,15 +9569,15 @@
         <f>C3-B3</f>
         <v>1.8865740740740742E-3</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="53">
         <f>D3*86400</f>
         <v>163</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="62">
+        <v>49</v>
+      </c>
+      <c r="I3" s="58">
         <f>MIN(E3:E14)</f>
         <v>86</v>
       </c>
@@ -9581,14 +9596,14 @@
         <f t="shared" ref="D4:D14" si="0">C4-B4</f>
         <v>1.6203703703703703E-3</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="53">
         <f t="shared" ref="E4:E14" si="1">D4*86400</f>
         <v>140</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="62">
+        <v>50</v>
+      </c>
+      <c r="I4" s="58">
         <f>MAX(E3:E14)</f>
         <v>315.99999999999994</v>
       </c>
@@ -9607,14 +9622,14 @@
         <f t="shared" si="0"/>
         <v>9.9537037037037042E-4</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="53">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="62">
+        <v>48</v>
+      </c>
+      <c r="I5" s="58">
         <f>AVERAGE(E3:E14)</f>
         <v>155.91666666666666</v>
       </c>
@@ -9633,7 +9648,7 @@
         <f t="shared" si="0"/>
         <v>2.3842592592592596E-3</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="53">
         <f t="shared" si="1"/>
         <v>206.00000000000003</v>
       </c>
@@ -9652,7 +9667,7 @@
         <f t="shared" si="0"/>
         <v>3.657407407407407E-3</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="53">
         <f t="shared" si="1"/>
         <v>315.99999999999994</v>
       </c>
@@ -9671,7 +9686,7 @@
         <f t="shared" si="0"/>
         <v>1.8171296296296299E-3</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="53">
         <f t="shared" si="1"/>
         <v>157.00000000000003</v>
       </c>
@@ -9690,7 +9705,7 @@
         <f t="shared" si="0"/>
         <v>1.5277777777777781E-3</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="53">
         <f t="shared" si="1"/>
         <v>132.00000000000003</v>
       </c>
@@ -9709,7 +9724,7 @@
         <f t="shared" si="0"/>
         <v>1.5277777777777776E-3</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="53">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
@@ -9728,7 +9743,7 @@
         <f t="shared" si="0"/>
         <v>2.6851851851851854E-3</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="53">
         <f t="shared" si="1"/>
         <v>232.00000000000003</v>
       </c>
@@ -9747,7 +9762,7 @@
         <f t="shared" si="0"/>
         <v>1.145833333333332E-3</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="53">
         <f t="shared" si="1"/>
         <v>98.999999999999886</v>
       </c>
@@ -9766,7 +9781,7 @@
         <f t="shared" si="0"/>
         <v>1.2152777777777769E-3</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="53">
         <f t="shared" si="1"/>
         <v>104.99999999999993</v>
       </c>
@@ -9785,7 +9800,7 @@
         <f t="shared" si="0"/>
         <v>1.1921296296296289E-3</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="53">
         <f t="shared" si="1"/>
         <v>102.99999999999994</v>
       </c>
@@ -9871,95 +9886,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="C3" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="D3" s="60" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="66">
+        <v>56</v>
+      </c>
+      <c r="B4" s="62">
         <v>513</v>
       </c>
-      <c r="C4" s="66">
+      <c r="C4" s="62">
         <v>521.81700000000001</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="62">
         <f>ABS(B4-C4)</f>
         <v>8.8170000000000073</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="66">
+        <v>57</v>
+      </c>
+      <c r="B5" s="62">
         <v>45.33</v>
       </c>
-      <c r="C5" s="66">
+      <c r="C5" s="62">
         <v>45.03</v>
       </c>
-      <c r="D5" s="66">
+      <c r="D5" s="62">
         <f>ABS(B5-C5)</f>
         <v>0.29999999999999716</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9968,10 +9983,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:D96"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75:K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9980,1114 +9995,1320 @@
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>56</v>
+      <c r="A2" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="68">
+      <c r="A3" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C3" s="68">
+      <c r="C3" s="64">
         <v>22.32</v>
       </c>
-      <c r="D3" s="68">
+      <c r="D3" s="64">
         <f>ABS(B3-C3)</f>
         <v>21.655000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="68">
+      <c r="A4" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="64">
         <v>0.45</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="64">
         <v>12.948</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="64">
         <f t="shared" ref="D4:D10" si="0">ABS(B4-C4)</f>
         <v>12.498000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="64">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="C5" s="64">
+        <v>13.06</v>
+      </c>
+      <c r="D5" s="64">
+        <f t="shared" si="0"/>
+        <v>12.375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="68">
-        <v>0.68500000000000005</v>
-      </c>
-      <c r="C5" s="68">
-        <v>13.06</v>
-      </c>
-      <c r="D5" s="68">
-        <f t="shared" si="0"/>
-        <v>12.375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="B6" s="64">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="C6" s="64">
+        <v>13.21</v>
+      </c>
+      <c r="D6" s="64">
+        <f t="shared" si="0"/>
+        <v>12.295000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="68">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="C6" s="68">
-        <v>13.21</v>
-      </c>
-      <c r="D6" s="68">
-        <f t="shared" si="0"/>
-        <v>12.295000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="B7" s="64">
+        <v>45.341999999999999</v>
+      </c>
+      <c r="C7" s="64">
+        <v>45.375</v>
+      </c>
+      <c r="D7" s="64">
+        <f t="shared" si="0"/>
+        <v>3.3000000000001251E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="68">
-        <v>45.341999999999999</v>
-      </c>
-      <c r="C7" s="68">
-        <v>45.375</v>
-      </c>
-      <c r="D7" s="68">
-        <f t="shared" si="0"/>
-        <v>3.3000000000001251E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="B8" s="64">
+        <v>38.167000000000002</v>
+      </c>
+      <c r="C8" s="64">
+        <v>814.08600000000001</v>
+      </c>
+      <c r="D8" s="64">
+        <f t="shared" si="0"/>
+        <v>775.91899999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="68">
-        <v>38.167000000000002</v>
-      </c>
-      <c r="C8" s="68">
-        <v>814.08600000000001</v>
-      </c>
-      <c r="D8" s="68">
-        <f t="shared" si="0"/>
-        <v>775.91899999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="B9" s="64">
+        <v>521.375</v>
+      </c>
+      <c r="C9" s="64">
+        <v>1294.6590000000001</v>
+      </c>
+      <c r="D9" s="64">
+        <f t="shared" si="0"/>
+        <v>773.28400000000011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="68">
-        <v>521.375</v>
-      </c>
-      <c r="C9" s="68">
-        <v>1294.6590000000001</v>
-      </c>
-      <c r="D9" s="68">
-        <f t="shared" si="0"/>
-        <v>773.28400000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="68">
+      <c r="B10" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="64">
         <v>0.65600000000000003</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="64">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="64" t="s">
+      <c r="A15" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="64" t="s">
-        <v>56</v>
+      <c r="C15" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="68">
+      <c r="A16" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="64">
         <v>1.663</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="64">
         <f>ABS(B16-C16)</f>
         <v>0.998</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="68">
+      <c r="A17" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="64">
         <v>0.45</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="64">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="D17" s="68">
+      <c r="D17" s="64">
         <f t="shared" ref="D17:D23" si="1">ABS(B17-C17)</f>
         <v>0.37270000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="64">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="C18" s="64">
+        <v>1.022</v>
+      </c>
+      <c r="D18" s="64">
+        <f t="shared" si="1"/>
+        <v>0.33699999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="68">
-        <v>0.68500000000000005</v>
-      </c>
-      <c r="C18" s="68">
-        <v>1.022</v>
-      </c>
-      <c r="D18" s="68">
-        <f t="shared" si="1"/>
-        <v>0.33699999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
+      <c r="B19" s="64">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="C19" s="64">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="D19" s="64">
+        <f t="shared" si="1"/>
+        <v>0.37999999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="68">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="C19" s="68">
-        <v>1.2949999999999999</v>
-      </c>
-      <c r="D19" s="68">
-        <f t="shared" si="1"/>
-        <v>0.37999999999999989</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="B20" s="64">
+        <v>45.341999999999999</v>
+      </c>
+      <c r="C20" s="64">
+        <v>45.381999999999998</v>
+      </c>
+      <c r="D20" s="64">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999147E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="68">
-        <v>45.341999999999999</v>
-      </c>
-      <c r="C20" s="68">
-        <v>45.381999999999998</v>
-      </c>
-      <c r="D20" s="68">
-        <f t="shared" si="1"/>
-        <v>3.9999999999999147E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
+      <c r="B21" s="64">
+        <v>38.167000000000002</v>
+      </c>
+      <c r="C21" s="64">
+        <v>53.220999999999997</v>
+      </c>
+      <c r="D21" s="64">
+        <f t="shared" si="1"/>
+        <v>15.053999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="68">
-        <v>38.167000000000002</v>
-      </c>
-      <c r="C21" s="68">
-        <v>53.220999999999997</v>
-      </c>
-      <c r="D21" s="68">
-        <f t="shared" si="1"/>
-        <v>15.053999999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="67" t="s">
+      <c r="B22" s="64">
+        <v>521.375</v>
+      </c>
+      <c r="C22" s="64">
+        <v>535.75099999999998</v>
+      </c>
+      <c r="D22" s="64">
+        <f t="shared" si="1"/>
+        <v>14.375999999999976</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="68">
-        <v>521.375</v>
-      </c>
-      <c r="C22" s="68">
-        <v>535.75099999999998</v>
-      </c>
-      <c r="D22" s="68">
-        <f t="shared" si="1"/>
-        <v>14.375999999999976</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="68">
+      <c r="B23" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C23" s="68">
+      <c r="C23" s="64">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D23" s="68">
+      <c r="D23" s="64">
         <f t="shared" si="1"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>56</v>
+      <c r="D28" s="60" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="68">
+      <c r="A29" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C29" s="68">
+      <c r="C29" s="64">
         <v>1.26</v>
       </c>
-      <c r="D29" s="68">
+      <c r="D29" s="64">
         <f>ABS(B29-C29)</f>
         <v>0.59499999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="68">
+      <c r="A30" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="64">
         <v>0.45</v>
       </c>
-      <c r="C30" s="68">
+      <c r="C30" s="64">
         <v>0.52600000000000002</v>
       </c>
-      <c r="D30" s="68">
+      <c r="D30" s="64">
         <f t="shared" ref="D30:D36" si="2">ABS(B30-C30)</f>
         <v>7.6000000000000012E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="68">
+      <c r="A31" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C31" s="68">
+      <c r="C31" s="64">
         <v>0.75900000000000001</v>
       </c>
-      <c r="D31" s="68">
+      <c r="D31" s="64">
         <f t="shared" si="2"/>
         <v>7.3999999999999955E-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="68">
+      <c r="A32" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C32" s="68">
+      <c r="C32" s="64">
         <v>1.0149999999999999</v>
       </c>
-      <c r="D32" s="68">
+      <c r="D32" s="64">
         <f t="shared" si="2"/>
         <v>9.9999999999999867E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="68">
+      <c r="A33" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C33" s="68">
+      <c r="C33" s="64">
         <v>47.435000000000002</v>
       </c>
-      <c r="D33" s="68">
+      <c r="D33" s="64">
         <f t="shared" si="2"/>
         <v>2.0930000000000035</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="68">
+      <c r="A34" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C34" s="68">
+      <c r="C34" s="64">
         <v>49.777999999999999</v>
       </c>
-      <c r="D34" s="68">
+      <c r="D34" s="64">
         <f t="shared" si="2"/>
         <v>11.610999999999997</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="68">
+      <c r="A35" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="64">
         <v>521.375</v>
       </c>
-      <c r="C35" s="68">
+      <c r="C35" s="64">
         <v>535.31600000000003</v>
       </c>
-      <c r="D35" s="68">
+      <c r="D35" s="64">
         <f t="shared" si="2"/>
         <v>13.941000000000031</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="68">
+      <c r="A36" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C36" s="68">
+      <c r="C36" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D36" s="68">
+      <c r="D36" s="64">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>56</v>
+      <c r="A40" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="68">
+      <c r="A41" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C41" s="68">
+      <c r="C41" s="64">
         <v>2.294</v>
       </c>
-      <c r="D41" s="68">
+      <c r="D41" s="64">
         <f>ABS(B41-C41)</f>
         <v>1.629</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="68">
+      <c r="A42" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="64">
         <v>0.45</v>
       </c>
-      <c r="C42" s="68">
+      <c r="C42" s="64">
         <v>0.88200000000000001</v>
       </c>
-      <c r="D42" s="68">
+      <c r="D42" s="64">
         <f t="shared" ref="D42:D48" si="3">ABS(B42-C42)</f>
         <v>0.432</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="68">
+      <c r="A43" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C43" s="68">
+      <c r="C43" s="64">
         <v>0.95899999999999996</v>
       </c>
-      <c r="D43" s="68">
+      <c r="D43" s="64">
         <f t="shared" si="3"/>
         <v>0.27399999999999991</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="68">
+      <c r="A44" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C44" s="68">
+      <c r="C44" s="64">
         <v>1.27</v>
       </c>
-      <c r="D44" s="68">
+      <c r="D44" s="64">
         <f t="shared" si="3"/>
         <v>0.35499999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="68">
+      <c r="A45" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C45" s="68">
+      <c r="C45" s="64">
         <v>50.430999999999997</v>
       </c>
-      <c r="D45" s="68">
+      <c r="D45" s="64">
         <f t="shared" si="3"/>
         <v>5.0889999999999986</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="68">
+      <c r="A46" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C46" s="68">
+      <c r="C46" s="64">
         <v>67.444000000000003</v>
       </c>
-      <c r="D46" s="68">
+      <c r="D46" s="64">
         <f t="shared" si="3"/>
         <v>29.277000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="68">
+      <c r="A47" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="64">
         <v>521.375</v>
       </c>
-      <c r="C47" s="68">
+      <c r="C47" s="64">
         <v>556.03099999999995</v>
       </c>
-      <c r="D47" s="68">
+      <c r="D47" s="64">
         <f t="shared" si="3"/>
         <v>34.655999999999949</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="68">
+      <c r="A48" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C48" s="68"/>
-      <c r="D48" s="68">
+      <c r="C48" s="64">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D48" s="64">
         <f t="shared" si="3"/>
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" s="68">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C52" s="68">
+      <c r="C52" s="64">
         <v>7.468</v>
       </c>
-      <c r="D52" s="68">
+      <c r="D52" s="64">
         <f>ABS(B52-C52)</f>
         <v>6.8029999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="68">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="64">
         <v>0.45</v>
       </c>
-      <c r="C53" s="68">
+      <c r="C53" s="64">
         <v>1.984</v>
       </c>
-      <c r="D53" s="68">
+      <c r="D53" s="64">
         <f t="shared" ref="D53:D59" si="4">ABS(B53-C53)</f>
         <v>1.534</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="68">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C54" s="68">
+      <c r="C54" s="64">
         <v>2.2330000000000001</v>
       </c>
-      <c r="D54" s="68">
+      <c r="D54" s="64">
         <f t="shared" si="4"/>
         <v>1.548</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="68">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C55" s="68">
+      <c r="C55" s="64">
         <v>2.36</v>
       </c>
-      <c r="D55" s="68">
+      <c r="D55" s="64">
         <f t="shared" si="4"/>
         <v>1.4449999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="68">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C56" s="68">
+      <c r="C56" s="64">
         <v>54.411000000000001</v>
       </c>
-      <c r="D56" s="68">
+      <c r="D56" s="64">
         <f t="shared" si="4"/>
         <v>9.0690000000000026</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="68">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C57" s="68">
+      <c r="C57" s="64">
         <v>108.753</v>
       </c>
-      <c r="D57" s="68">
+      <c r="D57" s="64">
         <f t="shared" si="4"/>
         <v>70.585999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="68">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="64">
         <v>521.375</v>
       </c>
-      <c r="C58" s="68">
+      <c r="C58" s="64">
         <v>601.15300000000002</v>
       </c>
-      <c r="D58" s="68">
+      <c r="D58" s="64">
         <f t="shared" si="4"/>
         <v>79.77800000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="68">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C59" s="68">
+      <c r="C59" s="64">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D59" s="68">
+      <c r="D59" s="64">
         <f t="shared" si="4"/>
         <v>2.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D63" s="64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" s="68">
+        <v>73</v>
+      </c>
+      <c r="H62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="I63" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="J63" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="K63" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="L63" s="60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C64" s="68">
+      <c r="C64" s="64">
         <v>13.323</v>
       </c>
-      <c r="D64" s="68">
+      <c r="D64" s="64">
         <f>ABS(B64-C64)</f>
         <v>12.658000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="68">
+      <c r="H64" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="I64" s="64">
+        <v>1.26</v>
+      </c>
+      <c r="J64" s="64">
+        <v>2.294</v>
+      </c>
+      <c r="K64" s="64">
+        <v>7.468</v>
+      </c>
+      <c r="L64" s="64">
+        <v>13.323</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="64">
         <v>0.45</v>
       </c>
-      <c r="C65" s="68">
+      <c r="C65" s="64">
         <v>5.069</v>
       </c>
-      <c r="D65" s="68">
+      <c r="D65" s="64">
         <f t="shared" ref="D65:D71" si="5">ABS(B65-C65)</f>
         <v>4.6189999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="68">
+      <c r="H65" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="I65" s="64">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="J65" s="64">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="K65" s="64">
+        <v>1.984</v>
+      </c>
+      <c r="L65" s="64">
+        <v>5.069</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C66" s="68">
+      <c r="C66" s="64">
         <v>5.516</v>
       </c>
-      <c r="D66" s="68">
+      <c r="D66" s="64">
         <f t="shared" si="5"/>
         <v>4.8309999999999995</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" s="68">
+      <c r="H66" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="I66" s="64">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="J66" s="64">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="K66" s="64">
+        <v>2.2330000000000001</v>
+      </c>
+      <c r="L66" s="64">
+        <v>5.516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C67" s="68">
+      <c r="C67" s="64">
         <v>5.6959999999999997</v>
       </c>
-      <c r="D67" s="68">
+      <c r="D67" s="64">
         <f t="shared" si="5"/>
         <v>4.7809999999999997</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="68">
+      <c r="H67" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" s="64">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="J67" s="64">
+        <v>1.27</v>
+      </c>
+      <c r="K67" s="64">
+        <v>2.36</v>
+      </c>
+      <c r="L67" s="64">
+        <v>5.6959999999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C68" s="68">
+      <c r="C68" s="64">
         <v>58.982999999999997</v>
       </c>
-      <c r="D68" s="68">
+      <c r="D68" s="64">
         <f t="shared" si="5"/>
         <v>13.640999999999998</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="68">
+      <c r="H68" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="I68" s="64">
+        <v>47.435000000000002</v>
+      </c>
+      <c r="J68" s="64">
+        <v>50.430999999999997</v>
+      </c>
+      <c r="K68" s="64">
+        <v>54.411000000000001</v>
+      </c>
+      <c r="L68" s="64">
+        <v>58.982999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C69" s="68">
+      <c r="C69" s="64">
         <v>220.26499999999999</v>
       </c>
-      <c r="D69" s="68">
+      <c r="D69" s="64">
         <f t="shared" si="5"/>
         <v>182.09799999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="68">
+      <c r="H69" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="I69" s="64">
+        <v>49.777999999999999</v>
+      </c>
+      <c r="J69" s="64">
+        <v>67.444000000000003</v>
+      </c>
+      <c r="K69" s="64">
+        <v>108.753</v>
+      </c>
+      <c r="L69" s="64">
+        <v>220.26499999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="64">
         <v>521.375</v>
       </c>
-      <c r="C70" s="68">
+      <c r="C70" s="64">
         <v>717.15800000000002</v>
       </c>
-      <c r="D70" s="68">
+      <c r="D70" s="64">
         <f t="shared" si="5"/>
         <v>195.78300000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="68">
+      <c r="H70" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" s="64">
+        <v>535.31600000000003</v>
+      </c>
+      <c r="J70" s="64">
+        <v>556.03099999999995</v>
+      </c>
+      <c r="K70" s="64">
+        <v>601.15300000000002</v>
+      </c>
+      <c r="L70" s="64">
+        <v>717.15800000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C71" s="68">
+      <c r="C71" s="64">
         <v>0.10199999999999999</v>
       </c>
-      <c r="D71" s="68">
+      <c r="D71" s="64">
         <f t="shared" si="5"/>
         <v>9.5999999999999988E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D75" s="64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B76" s="68">
+      <c r="H71" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="I71" s="64">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J71" s="64">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K71" s="64">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="L71" s="64">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="I75" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="J75" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="K75" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="L75" s="72"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C76" s="68">
+      <c r="C76" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="D76" s="68">
+      <c r="D76" s="64">
         <f>ABS(B76-C76)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B77" s="68">
+      <c r="H76" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="I76" s="64">
+        <f>0.006*100</f>
+        <v>0.6</v>
+      </c>
+      <c r="J76" s="64">
+        <f>0.013*100</f>
+        <v>1.3</v>
+      </c>
+      <c r="K76" s="64">
+        <f>0.004*100</f>
+        <v>0.4</v>
+      </c>
+      <c r="L76" s="71"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" s="64">
         <v>0.45</v>
       </c>
-      <c r="C77" s="68">
+      <c r="C77" s="64">
         <v>0.45</v>
       </c>
-      <c r="D77" s="68">
+      <c r="D77" s="64">
         <f t="shared" ref="D77:D83" si="6">ABS(B77-C77)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="68">
+      <c r="H77" s="70"/>
+      <c r="I77" s="71"/>
+      <c r="J77" s="71"/>
+      <c r="K77" s="71"/>
+      <c r="L77" s="71"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C78" s="68">
+      <c r="C78" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="D78" s="68">
+      <c r="D78" s="64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B79" s="68">
+      <c r="H78" s="70"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="71"/>
+      <c r="K78" s="71"/>
+      <c r="L78" s="71"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C79" s="68">
+      <c r="C79" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="D79" s="68">
+      <c r="D79" s="64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B80" s="68">
+      <c r="H79" s="70"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
+      <c r="K79" s="71"/>
+      <c r="L79" s="71"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C80" s="68">
+      <c r="C80" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="D80" s="68">
+      <c r="D80" s="64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B81" s="68">
+      <c r="H80" s="70"/>
+      <c r="I80" s="71"/>
+      <c r="J80" s="71"/>
+      <c r="K80" s="71"/>
+      <c r="L80" s="71"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C81" s="68">
+      <c r="C81" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="D81" s="68">
+      <c r="D81" s="64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B82" s="68">
+      <c r="H81" s="70"/>
+      <c r="I81" s="71"/>
+      <c r="J81" s="71"/>
+      <c r="K81" s="71"/>
+      <c r="L81" s="71"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B82" s="64">
         <v>521.375</v>
       </c>
-      <c r="C82" s="68">
+      <c r="C82" s="64">
         <v>521.375</v>
       </c>
-      <c r="D82" s="68">
+      <c r="D82" s="64">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B83" s="68">
+      <c r="H82" s="70"/>
+      <c r="I82" s="71"/>
+      <c r="J82" s="71"/>
+      <c r="K82" s="71"/>
+      <c r="L82" s="71"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B83" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C83" s="68">
+      <c r="C83" s="64">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D83" s="68">
+      <c r="D83" s="64">
         <f t="shared" si="6"/>
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="70" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B88" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C88" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D88" s="64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B89" s="68">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C88" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" s="60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="C89" s="68">
+      <c r="C89" s="64">
         <v>0.66500000000000004</v>
       </c>
-      <c r="D89" s="68">
+      <c r="D89" s="64">
         <f>ABS(B89-C89)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B90" s="68">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="64">
         <v>0.45</v>
       </c>
-      <c r="C90" s="68">
+      <c r="C90" s="64">
         <v>0.45</v>
       </c>
-      <c r="D90" s="68">
+      <c r="D90" s="64">
         <f t="shared" ref="D90:D96" si="7">ABS(B90-C90)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B91" s="68">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C91" s="68">
+      <c r="C91" s="64">
         <v>0.68500000000000005</v>
       </c>
-      <c r="D91" s="68">
+      <c r="D91" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="B92" s="68">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="C92" s="68">
+      <c r="C92" s="64">
         <v>0.91500000000000004</v>
       </c>
-      <c r="D92" s="68">
+      <c r="D92" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B93" s="68">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B93" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="C93" s="68">
+      <c r="C93" s="64">
         <v>45.341999999999999</v>
       </c>
-      <c r="D93" s="68">
+      <c r="D93" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" s="68">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B94" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="C94" s="68">
+      <c r="C94" s="64">
         <v>38.167000000000002</v>
       </c>
-      <c r="D94" s="68">
+      <c r="D94" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B95" s="68">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B95" s="64">
         <v>521.375</v>
       </c>
-      <c r="C95" s="68">
+      <c r="C95" s="64">
         <v>521.375</v>
       </c>
-      <c r="D95" s="68">
+      <c r="D95" s="64">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B96" s="68">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" s="64">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C96" s="68">
+      <c r="C96" s="64">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D96" s="68">
+      <c r="D96" s="64">
         <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>

</xml_diff>